<commit_message>
rill-analysis: Liantiao for luopan
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="89">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,10 +160,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>searchTrendByCondition.action</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>posIdString</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -313,6 +309,102 @@
   </si>
   <si>
     <t>00：00-01：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>searchRealTimeTrendByCondition.action</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01：00-02：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02：00-03：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03：00-04：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>04：00-05：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>05：00-06：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>06：00-07：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>07：00-08：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>08：00-09：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>09：00-10：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10：00-11：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11：00-12：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12：00-13：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13：00-14：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14：00-15：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15：00-16：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17：00-18：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18：00-19：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>21：00-22：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22：00-23：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>23：00-24：00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -747,7 +839,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -802,9 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -829,19 +918,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -850,13 +945,7 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -868,11 +957,17 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1628,11 +1723,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83113472"/>
-        <c:axId val="83115008"/>
+        <c:axId val="85749120"/>
+        <c:axId val="85755008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83113472"/>
+        <c:axId val="85749120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,14 +1736,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83115008"/>
+        <c:crossAx val="85755008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83115008"/>
+        <c:axId val="85755008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1752,7 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83113472"/>
+        <c:crossAx val="85749120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1675,7 +1770,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000711" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000711" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000766" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000766" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1692,7 +1787,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -2019,9 +2114,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Y51"/>
+  <dimension ref="B1:AA51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -2029,1484 +2124,1458 @@
     <col min="2" max="2" width="0.75" customWidth="1"/>
     <col min="3" max="12" width="6.125" customWidth="1"/>
     <col min="13" max="13" width="1.125" customWidth="1"/>
-    <col min="14" max="16" width="6.125" customWidth="1"/>
-    <col min="17" max="17" width="1.5" customWidth="1"/>
-    <col min="18" max="18" width="8.625" customWidth="1"/>
-    <col min="19" max="19" width="1.5" customWidth="1"/>
-    <col min="20" max="22" width="6.125" customWidth="1"/>
-    <col min="23" max="23" width="1.5" customWidth="1"/>
-    <col min="24" max="24" width="8.625" customWidth="1"/>
+    <col min="14" max="17" width="6.125" customWidth="1"/>
+    <col min="18" max="18" width="1.5" customWidth="1"/>
+    <col min="19" max="19" width="8.625" customWidth="1"/>
+    <col min="20" max="20" width="1.5" customWidth="1"/>
+    <col min="21" max="24" width="6.125" customWidth="1"/>
     <col min="25" max="25" width="1.5" customWidth="1"/>
+    <col min="26" max="26" width="8.625" customWidth="1"/>
+    <col min="27" max="27" width="1.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="3.75" customHeight="1">
-      <c r="Q1" s="5"/>
-    </row>
-    <row r="2" spans="2:17">
-      <c r="B2" s="40" t="str">
+    <row r="1" spans="2:18" ht="3.75" customHeight="1">
+      <c r="R1" s="5"/>
+    </row>
+    <row r="2" spans="2:18">
+      <c r="B2" s="27" t="str">
         <f>_input!$A2&amp;"+"&amp;_input!$A3&amp;"+趋势图"</f>
         <v>商业产品线+分析指标+趋势图</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="B4" s="18" t="str">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="R3" s="5"/>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="26" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="2"/>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="2:17" ht="3" customHeight="1">
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="2:17">
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="2:17">
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="2:17">
-      <c r="Q9" s="5"/>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="Q10" s="5"/>
-    </row>
-    <row r="11" spans="2:17">
-      <c r="Q11" s="5"/>
-    </row>
-    <row r="12" spans="2:17">
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="Q13" s="5"/>
-    </row>
-    <row r="14" spans="2:17">
-      <c r="Q14" s="5"/>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="Q15" s="5"/>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="Q16" s="5"/>
-    </row>
-    <row r="17" spans="2:25">
-      <c r="Q17" s="5"/>
-    </row>
-    <row r="18" spans="2:25">
-      <c r="Q18" s="5"/>
-    </row>
-    <row r="19" spans="2:25">
-      <c r="Q19" s="5"/>
-    </row>
-    <row r="20" spans="2:25">
-      <c r="Q20" s="5"/>
-    </row>
-    <row r="21" spans="2:25">
-      <c r="Q21" s="5"/>
-    </row>
-    <row r="22" spans="2:25">
-      <c r="Q22" s="5"/>
-    </row>
-    <row r="23" spans="2:25">
-      <c r="Q23" s="5"/>
-    </row>
-    <row r="24" spans="2:25">
-      <c r="B24" s="40" t="str">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" spans="2:18" ht="3" customHeight="1">
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="R6" s="5"/>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="R7" s="5"/>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="R8" s="5"/>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="R10" s="5"/>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="R11" s="5"/>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="R12" s="5"/>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="R13" s="5"/>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="R14" s="5"/>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="R15" s="5"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="R16" s="5"/>
+    </row>
+    <row r="17" spans="2:27">
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="2:27">
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="2:27">
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="2:27">
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="2:27">
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="2:27">
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="2:27">
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="2:27">
+      <c r="B24" s="27" t="str">
         <f>_input!$B3&amp;"分小时数据表"</f>
         <v>点击消费分小时数据表</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="Q24" s="5"/>
-      <c r="U24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:25" ht="3.75" customHeight="1"/>
-    <row r="26" spans="2:25" ht="3" customHeight="1">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-    </row>
-    <row r="27" spans="2:25" ht="35.25" customHeight="1">
-      <c r="B27" s="36" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="R24" s="5"/>
+      <c r="W24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" ht="3.75" customHeight="1"/>
+    <row r="26" spans="2:27" ht="3" customHeight="1">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+    </row>
+    <row r="27" spans="2:27" ht="35.25" customHeight="1">
+      <c r="B27" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="33" t="s">
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="36" t="s">
+      <c r="O27" s="28"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="U27" s="34"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="39"/>
-    </row>
-    <row r="28" spans="2:25">
-      <c r="B28" s="26"/>
-      <c r="C28" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29">
+      <c r="V27" s="28"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
+      <c r="AA27" s="38"/>
+    </row>
+    <row r="28" spans="2:27">
+      <c r="B28" s="25"/>
+      <c r="C28" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="39">
         <f>_input!$B5</f>
         <v>3344110</v>
       </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="30"/>
-      <c r="M28" s="25"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="31">
         <f>_input!$C5</f>
         <v>3224110</v>
       </c>
       <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" s="24">
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S28" s="23">
         <f>_input!$F5</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S28" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T28" s="31">
+      <c r="T28" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U28" s="31">
         <f>_input!$D5</f>
         <v>3334440</v>
       </c>
-      <c r="U28" s="32"/>
       <c r="V28" s="32"/>
-      <c r="W28" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X28" s="24">
+      <c r="W28" s="33"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z28" s="23">
         <f>_input!$G5</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y28" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="2:25">
-      <c r="B29" s="26"/>
-      <c r="C29" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29">
+      <c r="AA28" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27">
+      <c r="B29" s="25"/>
+      <c r="C29" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="39">
         <f>_input!$B6</f>
         <v>3323110</v>
       </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="25"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="24"/>
       <c r="N29" s="31">
         <f>_input!$C6</f>
         <v>4343110</v>
       </c>
       <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R29" s="24">
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S29" s="23">
         <f>_input!$F6</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="S29" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T29" s="31">
+      <c r="T29" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U29" s="31">
         <f>_input!$D6</f>
         <v>3323440</v>
       </c>
-      <c r="U29" s="32"/>
       <c r="V29" s="32"/>
-      <c r="W29" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X29" s="24">
+      <c r="W29" s="33"/>
+      <c r="X29" s="33"/>
+      <c r="Y29" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z29" s="23">
         <f>_input!$G6</f>
         <v>-9.9294706689456724E-5</v>
       </c>
-      <c r="Y29" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="2:25">
-      <c r="B30" s="26"/>
-      <c r="C30" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29">
+      <c r="AA29" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27">
+      <c r="B30" s="25"/>
+      <c r="C30" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="39">
         <f>_input!$B7</f>
         <v>3344110</v>
       </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="25"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="24"/>
       <c r="N30" s="31">
         <f>_input!$C7</f>
         <v>3224110</v>
       </c>
       <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" s="24">
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S30" s="23">
         <f>_input!$F7</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S30" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T30" s="31">
+      <c r="T30" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" s="31">
         <f>_input!$D7</f>
         <v>3324440</v>
       </c>
-      <c r="U30" s="32"/>
       <c r="V30" s="32"/>
-      <c r="W30" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X30" s="24">
+      <c r="W30" s="33"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z30" s="23">
         <f>_input!$G7</f>
         <v>5.9167859850079996E-3</v>
       </c>
-      <c r="Y30" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="2:25">
-      <c r="B31" s="26"/>
-      <c r="C31" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="29">
+      <c r="AA30" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27">
+      <c r="B31" s="25"/>
+      <c r="C31" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="39">
         <f>_input!$B8</f>
         <v>3344110</v>
       </c>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="25"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="24"/>
       <c r="N31" s="31">
         <f>_input!$C8</f>
         <v>3224110</v>
       </c>
       <c r="O31" s="32"/>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R31" s="24">
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S31" s="23">
         <f>_input!$F8</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S31" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T31" s="31">
+      <c r="T31" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U31" s="31">
         <f>_input!$D8</f>
         <v>3334440</v>
       </c>
-      <c r="U31" s="32"/>
       <c r="V31" s="32"/>
-      <c r="W31" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X31" s="24">
+      <c r="W31" s="33"/>
+      <c r="X31" s="33"/>
+      <c r="Y31" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z31" s="23">
         <f>_input!$G8</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y31" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25">
-      <c r="B32" s="26"/>
-      <c r="C32" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="29">
+      <c r="AA31" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27">
+      <c r="B32" s="25"/>
+      <c r="C32" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="39">
         <f>_input!$B9</f>
         <v>3344110</v>
       </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="25"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="24"/>
       <c r="N32" s="31">
         <f>_input!$C9</f>
         <v>3664110</v>
       </c>
       <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R32" s="24">
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S32" s="23">
         <f>_input!$F9</f>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="S32" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T32" s="31">
+      <c r="T32" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U32" s="31">
         <f>_input!$D9</f>
         <v>3244440</v>
       </c>
-      <c r="U32" s="32"/>
       <c r="V32" s="32"/>
-      <c r="W32" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X32" s="24">
+      <c r="W32" s="33"/>
+      <c r="X32" s="33"/>
+      <c r="Y32" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z32" s="23">
         <f>_input!$G9</f>
         <v>3.0720247561982994E-2</v>
       </c>
-      <c r="Y32" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="2:25">
-      <c r="B33" s="26"/>
-      <c r="C33" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="29">
+      <c r="AA32" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:27">
+      <c r="B33" s="25"/>
+      <c r="C33" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="39">
         <f>_input!$B10</f>
         <v>3344110</v>
       </c>
-      <c r="I33" s="30"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="25"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="24"/>
       <c r="N33" s="31">
         <f>_input!$C10</f>
         <v>3224110</v>
       </c>
       <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R33" s="24">
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S33" s="23">
         <f>_input!$F10</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S33" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T33" s="31">
+      <c r="T33" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U33" s="31">
         <f>_input!$D10</f>
         <v>3334440</v>
       </c>
-      <c r="U33" s="32"/>
       <c r="V33" s="32"/>
-      <c r="W33" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X33" s="24">
+      <c r="W33" s="33"/>
+      <c r="X33" s="33"/>
+      <c r="Y33" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z33" s="23">
         <f>_input!$G10</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y33" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="2:25">
-      <c r="B34" s="26"/>
-      <c r="C34" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29">
+      <c r="AA33" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:27">
+      <c r="B34" s="25"/>
+      <c r="C34" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="39">
         <f>_input!$B11</f>
         <v>4344110</v>
       </c>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="25"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="24"/>
       <c r="N34" s="31">
         <f>_input!$C11</f>
         <v>4324110</v>
       </c>
       <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R34" s="24">
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S34" s="23">
         <f>_input!$F11</f>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="S34" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T34" s="31">
+      <c r="T34" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U34" s="31">
         <f>_input!$D11</f>
         <v>3334440</v>
       </c>
-      <c r="U34" s="32"/>
       <c r="V34" s="32"/>
-      <c r="W34" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X34" s="24">
+      <c r="W34" s="33"/>
+      <c r="X34" s="33"/>
+      <c r="Y34" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z34" s="23">
         <f>_input!$G11</f>
         <v>0.30280047024387913</v>
       </c>
-      <c r="Y34" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="2:25">
-      <c r="B35" s="26"/>
-      <c r="C35" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="29">
+      <c r="AA34" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="2:27">
+      <c r="B35" s="25"/>
+      <c r="C35" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="39">
         <f>_input!$B12</f>
         <v>3344110</v>
       </c>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="25"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="24"/>
       <c r="N35" s="31">
         <f>_input!$C12</f>
         <v>3224110</v>
       </c>
       <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R35" s="24">
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S35" s="23">
         <f>_input!$F12</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S35" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T35" s="31">
+      <c r="T35" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U35" s="31">
         <f>_input!$D12</f>
         <v>3554440</v>
       </c>
-      <c r="U35" s="32"/>
       <c r="V35" s="32"/>
-      <c r="W35" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X35" s="24">
+      <c r="W35" s="33"/>
+      <c r="X35" s="33"/>
+      <c r="Y35" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z35" s="23">
         <f>_input!$G12</f>
         <v>-5.9173878304317973E-2</v>
       </c>
-      <c r="Y35" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="2:25">
-      <c r="B36" s="26"/>
-      <c r="C36" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="29">
+      <c r="AA35" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:27">
+      <c r="B36" s="25"/>
+      <c r="C36" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="39">
         <f>_input!$B13</f>
         <v>3344110</v>
       </c>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="25"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="24"/>
       <c r="N36" s="31">
         <f>_input!$C13</f>
         <v>3224110</v>
       </c>
       <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R36" s="24">
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S36" s="23">
         <f>_input!$F13</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S36" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T36" s="31">
+      <c r="T36" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U36" s="31">
         <f>_input!$D13</f>
         <v>3674440</v>
       </c>
-      <c r="U36" s="32"/>
       <c r="V36" s="32"/>
-      <c r="W36" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X36" s="24">
+      <c r="W36" s="33"/>
+      <c r="X36" s="33"/>
+      <c r="Y36" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z36" s="23">
         <f>_input!$G13</f>
         <v>-8.9899413243922921E-2</v>
       </c>
-      <c r="Y36" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="2:25">
-      <c r="B37" s="26"/>
-      <c r="C37" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29">
+      <c r="AA36" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:27">
+      <c r="B37" s="25"/>
+      <c r="C37" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="39">
         <f>_input!$B14</f>
         <v>3344110</v>
       </c>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="25"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="24"/>
       <c r="N37" s="31">
         <f>_input!$C14</f>
         <v>3224110</v>
       </c>
       <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R37" s="24">
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S37" s="23">
         <f>_input!$F14</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S37" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T37" s="31">
+      <c r="T37" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U37" s="31">
         <f>_input!$D14</f>
         <v>3334440</v>
       </c>
-      <c r="U37" s="32"/>
       <c r="V37" s="32"/>
-      <c r="W37" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X37" s="24">
+      <c r="W37" s="33"/>
+      <c r="X37" s="33"/>
+      <c r="Y37" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z37" s="23">
         <f>_input!$G14</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y37" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="2:25">
-      <c r="B38" s="26"/>
-      <c r="C38" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29">
+      <c r="AA37" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="2:27">
+      <c r="B38" s="25"/>
+      <c r="C38" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="39">
         <f>_input!$B15</f>
         <v>3344110</v>
       </c>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="25"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="24"/>
       <c r="N38" s="31">
         <f>_input!$C15</f>
         <v>3524110</v>
       </c>
       <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R38" s="24">
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S38" s="23">
         <f>_input!$F15</f>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="S38" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T38" s="31">
+      <c r="T38" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U38" s="31">
         <f>_input!$D15</f>
         <v>3544440</v>
       </c>
-      <c r="U38" s="32"/>
       <c r="V38" s="32"/>
-      <c r="W38" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X38" s="24">
+      <c r="W38" s="33"/>
+      <c r="X38" s="33"/>
+      <c r="Y38" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z38" s="23">
         <f>_input!$G15</f>
         <v>-5.65195066075318E-2</v>
       </c>
-      <c r="Y38" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="2:25">
-      <c r="B39" s="26"/>
-      <c r="C39" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="29">
+      <c r="AA38" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:27">
+      <c r="B39" s="25"/>
+      <c r="C39" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="39">
         <f>_input!$B16</f>
         <v>3344110</v>
       </c>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="25"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="24"/>
       <c r="N39" s="31">
         <f>_input!$C16</f>
         <v>3224110</v>
       </c>
       <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R39" s="24">
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S39" s="23">
         <f>_input!$F16</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S39" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T39" s="31">
+      <c r="T39" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U39" s="31">
         <f>_input!$D16</f>
         <v>3334440</v>
       </c>
-      <c r="U39" s="32"/>
       <c r="V39" s="32"/>
-      <c r="W39" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X39" s="24">
+      <c r="W39" s="33"/>
+      <c r="X39" s="33"/>
+      <c r="Y39" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z39" s="23">
         <f>_input!$G16</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y39" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:25">
-      <c r="B40" s="26"/>
-      <c r="C40" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="29">
+      <c r="AA39" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:27">
+      <c r="B40" s="25"/>
+      <c r="C40" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="39">
         <f>_input!$B17</f>
         <v>3344110</v>
       </c>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="25"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="24"/>
       <c r="N40" s="31">
         <f>_input!$C17</f>
         <v>3224110</v>
       </c>
       <c r="O40" s="32"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R40" s="24">
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S40" s="23">
         <f>_input!$F17</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S40" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T40" s="31">
+      <c r="T40" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U40" s="31">
         <f>_input!$D17</f>
         <v>3334440</v>
       </c>
-      <c r="U40" s="32"/>
       <c r="V40" s="32"/>
-      <c r="W40" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X40" s="24">
+      <c r="W40" s="33"/>
+      <c r="X40" s="33"/>
+      <c r="Y40" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z40" s="23">
         <f>_input!$G17</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y40" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="2:25">
-      <c r="B41" s="26"/>
-      <c r="C41" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29">
+      <c r="AA40" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:27">
+      <c r="B41" s="25"/>
+      <c r="C41" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="39">
         <f>_input!$B18</f>
         <v>3484110</v>
       </c>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="25"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="24"/>
       <c r="N41" s="31">
         <f>_input!$C18</f>
         <v>3224110</v>
       </c>
       <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R41" s="24">
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S41" s="23">
         <f>_input!$F18</f>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="S41" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T41" s="31">
+      <c r="T41" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U41" s="31">
         <f>_input!$D18</f>
         <v>3344440</v>
       </c>
-      <c r="U41" s="32"/>
       <c r="V41" s="32"/>
-      <c r="W41" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X41" s="24">
+      <c r="W41" s="33"/>
+      <c r="X41" s="33"/>
+      <c r="Y41" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z41" s="23">
         <f>_input!$G18</f>
         <v>4.1761849517407912E-2</v>
       </c>
-      <c r="Y41" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="2:25">
-      <c r="B42" s="26"/>
-      <c r="C42" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="29">
+      <c r="AA41" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:27">
+      <c r="B42" s="25"/>
+      <c r="C42" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="39">
         <f>_input!$B19</f>
         <v>3344110</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="25"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="24"/>
       <c r="N42" s="31">
         <f>_input!$C19</f>
         <v>3224110</v>
       </c>
       <c r="O42" s="32"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R42" s="24">
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S42" s="23">
         <f>_input!$F19</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S42" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T42" s="31">
+      <c r="T42" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U42" s="31">
         <f>_input!$D19</f>
         <v>3334440</v>
       </c>
-      <c r="U42" s="32"/>
       <c r="V42" s="32"/>
-      <c r="W42" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X42" s="24">
+      <c r="W42" s="33"/>
+      <c r="X42" s="33"/>
+      <c r="Y42" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z42" s="23">
         <f>_input!$G19</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y42" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="2:25">
-      <c r="B43" s="26"/>
-      <c r="C43" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="29">
+      <c r="AA42" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:27">
+      <c r="B43" s="25"/>
+      <c r="C43" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="39">
         <f>_input!$B20</f>
         <v>3344110</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
-      <c r="L43" s="30"/>
-      <c r="M43" s="25"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="24"/>
       <c r="N43" s="31">
         <f>_input!$C20</f>
         <v>3224110</v>
       </c>
       <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R43" s="24">
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S43" s="23">
         <f>_input!$F20</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T43" s="31">
+      <c r="T43" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U43" s="31">
         <f>_input!$D20</f>
         <v>3544440</v>
       </c>
-      <c r="U43" s="32"/>
       <c r="V43" s="32"/>
-      <c r="W43" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X43" s="24">
+      <c r="W43" s="33"/>
+      <c r="X43" s="33"/>
+      <c r="Y43" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z43" s="23">
         <f>_input!$G20</f>
         <v>-5.65195066075318E-2</v>
       </c>
-      <c r="Y43" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="2:25">
-      <c r="B44" s="26"/>
-      <c r="C44" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="29">
+      <c r="AA43" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27">
+      <c r="B44" s="25"/>
+      <c r="C44" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="39">
         <f>_input!$B21</f>
         <v>3344110</v>
       </c>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
-      <c r="M44" s="25"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="24"/>
       <c r="N44" s="31">
         <f>_input!$C21</f>
         <v>3434110</v>
       </c>
       <c r="O44" s="32"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R44" s="24">
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S44" s="23">
         <f>_input!$F21</f>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="S44" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T44" s="31">
+      <c r="T44" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U44" s="31">
         <f>_input!$D21</f>
         <v>3334440</v>
       </c>
-      <c r="U44" s="32"/>
       <c r="V44" s="32"/>
-      <c r="W44" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X44" s="24">
+      <c r="W44" s="33"/>
+      <c r="X44" s="33"/>
+      <c r="Y44" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z44" s="23">
         <f>_input!$G21</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y44" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="2:25">
-      <c r="B45" s="26"/>
-      <c r="C45" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="29">
+      <c r="AA44" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="2:27">
+      <c r="B45" s="25"/>
+      <c r="C45" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="39">
         <f>_input!$B22</f>
         <v>3344110</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
-      <c r="L45" s="30"/>
-      <c r="M45" s="25"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="24"/>
       <c r="N45" s="31">
         <f>_input!$C22</f>
         <v>3224110</v>
       </c>
       <c r="O45" s="32"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R45" s="24">
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S45" s="23">
         <f>_input!$F22</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S45" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T45" s="31">
+      <c r="T45" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U45" s="31">
         <f>_input!$D22</f>
         <v>3334440</v>
       </c>
-      <c r="U45" s="32"/>
       <c r="V45" s="32"/>
-      <c r="W45" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X45" s="24">
+      <c r="W45" s="33"/>
+      <c r="X45" s="33"/>
+      <c r="Y45" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z45" s="23">
         <f>_input!$G22</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y45" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="2:25">
-      <c r="B46" s="26"/>
-      <c r="C46" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="29">
+      <c r="AA45" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="2:27">
+      <c r="B46" s="25"/>
+      <c r="C46" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="39">
         <f>_input!$B23</f>
         <v>3344110</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="25"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="24"/>
       <c r="N46" s="31">
         <f>_input!$C23</f>
         <v>3224110</v>
       </c>
       <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R46" s="24">
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S46" s="23">
         <f>_input!$F23</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S46" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T46" s="31">
+      <c r="T46" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U46" s="31">
         <f>_input!$D23</f>
         <v>3334440</v>
       </c>
-      <c r="U46" s="32"/>
       <c r="V46" s="32"/>
-      <c r="W46" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X46" s="24">
+      <c r="W46" s="33"/>
+      <c r="X46" s="33"/>
+      <c r="Y46" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z46" s="23">
         <f>_input!$G23</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y46" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="2:25">
-      <c r="B47" s="26"/>
-      <c r="C47" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="29">
+      <c r="AA46" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="2:27">
+      <c r="B47" s="25"/>
+      <c r="C47" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="39">
         <f>_input!$B24</f>
         <v>2144110</v>
       </c>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="25"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="24"/>
       <c r="N47" s="31">
         <f>_input!$C24</f>
         <v>3224110</v>
       </c>
       <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R47" s="24">
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S47" s="23">
         <f>_input!$F24</f>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="S47" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T47" s="31">
+      <c r="T47" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U47" s="31">
         <f>_input!$D24</f>
         <v>3334440</v>
       </c>
-      <c r="U47" s="32"/>
       <c r="V47" s="32"/>
-      <c r="W47" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X47" s="24">
+      <c r="W47" s="33"/>
+      <c r="X47" s="33"/>
+      <c r="Y47" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z47" s="23">
         <f>_input!$G24</f>
         <v>-0.35698048247981673</v>
       </c>
-      <c r="Y47" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="2:25">
-      <c r="B48" s="26"/>
-      <c r="C48" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="29">
+      <c r="AA47" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27">
+      <c r="B48" s="25"/>
+      <c r="C48" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="39">
         <f>_input!$B25</f>
         <v>3344110</v>
       </c>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="25"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="24"/>
       <c r="N48" s="31">
         <f>_input!$C25</f>
         <v>3224110</v>
       </c>
       <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R48" s="24">
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S48" s="23">
         <f>_input!$F25</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S48" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T48" s="31">
+      <c r="T48" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U48" s="31">
         <f>_input!$D25</f>
         <v>3334440</v>
       </c>
-      <c r="U48" s="32"/>
       <c r="V48" s="32"/>
-      <c r="W48" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X48" s="24">
+      <c r="W48" s="33"/>
+      <c r="X48" s="33"/>
+      <c r="Y48" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z48" s="23">
         <f>_input!$G25</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y48" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="2:25">
-      <c r="B49" s="26"/>
-      <c r="C49" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="29">
+      <c r="AA48" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="2:27">
+      <c r="B49" s="25"/>
+      <c r="C49" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="39">
         <f>_input!$B26</f>
         <v>3344110</v>
       </c>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="25"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
+      <c r="M49" s="24"/>
       <c r="N49" s="31">
         <f>_input!$C26</f>
         <v>3224110</v>
       </c>
       <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R49" s="24">
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S49" s="23">
         <f>_input!$F26</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S49" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T49" s="31">
+      <c r="T49" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U49" s="31">
         <f>_input!$D26</f>
         <v>3334440</v>
       </c>
-      <c r="U49" s="32"/>
       <c r="V49" s="32"/>
-      <c r="W49" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X49" s="24">
+      <c r="W49" s="33"/>
+      <c r="X49" s="33"/>
+      <c r="Y49" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z49" s="23">
         <f>_input!$G26</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y49" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="2:25">
-      <c r="B50" s="26"/>
-      <c r="C50" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="29">
+      <c r="AA49" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="2:27">
+      <c r="B50" s="25"/>
+      <c r="C50" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="39">
         <f>_input!$B27</f>
         <v>3344110</v>
       </c>
-      <c r="I50" s="30"/>
-      <c r="J50" s="30"/>
-      <c r="K50" s="30"/>
-      <c r="L50" s="30"/>
-      <c r="M50" s="25"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
+      <c r="M50" s="24"/>
       <c r="N50" s="31">
         <f>_input!$C27</f>
         <v>3994110</v>
       </c>
       <c r="O50" s="32"/>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R50" s="24">
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S50" s="23">
         <f>_input!$F27</f>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="S50" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T50" s="31">
+      <c r="T50" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U50" s="31">
         <f>_input!$D27</f>
         <v>3334440</v>
       </c>
-      <c r="U50" s="32"/>
       <c r="V50" s="32"/>
-      <c r="W50" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X50" s="24">
+      <c r="W50" s="33"/>
+      <c r="X50" s="33"/>
+      <c r="Y50" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z50" s="23">
         <f>_input!$G27</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="Y50" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="2:25">
-      <c r="B51" s="26"/>
-      <c r="C51" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="29">
+      <c r="AA50" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:27">
+      <c r="B51" s="25"/>
+      <c r="C51" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="39">
         <f>_input!$B28</f>
         <v>3344110</v>
       </c>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="25"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="24"/>
       <c r="N51" s="31">
         <f>_input!$C28</f>
         <v>3224110</v>
       </c>
       <c r="O51" s="32"/>
-      <c r="P51" s="32"/>
-      <c r="Q51" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="R51" s="24">
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="S51" s="23">
         <f>_input!$F28</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="S51" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T51" s="31">
+      <c r="T51" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="U51" s="31">
         <f>_input!$D28</f>
         <v>3214440</v>
       </c>
-      <c r="U51" s="32"/>
       <c r="V51" s="32"/>
-      <c r="W51" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="X51" s="24">
+      <c r="W51" s="33"/>
+      <c r="X51" s="33"/>
+      <c r="Y51" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z51" s="23">
         <f>_input!$G28</f>
         <v>4.0339841465387494E-2</v>
       </c>
-      <c r="Y51" s="23" t="s">
-        <v>64</v>
+      <c r="AA51" s="22" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="102">
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="N27:S27"/>
-    <mergeCell ref="T27:Y27"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="T50:V50"/>
-    <mergeCell ref="T51:V51"/>
-    <mergeCell ref="T45:V45"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="T47:V47"/>
-    <mergeCell ref="T48:V48"/>
-    <mergeCell ref="T49:V49"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="N50:P50"/>
-    <mergeCell ref="N48:P48"/>
-    <mergeCell ref="N49:P49"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="N39:P39"/>
-    <mergeCell ref="N40:P40"/>
-    <mergeCell ref="N41:P41"/>
-    <mergeCell ref="N42:P42"/>
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="N37:P37"/>
-    <mergeCell ref="N43:P43"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="T28:V28"/>
-    <mergeCell ref="T29:V29"/>
-    <mergeCell ref="T30:V30"/>
-    <mergeCell ref="T31:V31"/>
-    <mergeCell ref="T32:V32"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="N47:P47"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="N32:P32"/>
-    <mergeCell ref="T43:V43"/>
-    <mergeCell ref="T44:V44"/>
-    <mergeCell ref="T38:V38"/>
-    <mergeCell ref="T39:V39"/>
-    <mergeCell ref="T40:V40"/>
-    <mergeCell ref="T41:V41"/>
-    <mergeCell ref="T42:V42"/>
-    <mergeCell ref="T33:V33"/>
-    <mergeCell ref="T34:V34"/>
-    <mergeCell ref="T35:V35"/>
-    <mergeCell ref="T36:V36"/>
-    <mergeCell ref="T37:V37"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="H49:L49"/>
+  <mergeCells count="103">
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="H50:L50"/>
@@ -3531,24 +3600,103 @@
     <mergeCell ref="C45:G45"/>
     <mergeCell ref="C46:G46"/>
     <mergeCell ref="C47:G47"/>
+    <mergeCell ref="U30:X30"/>
+    <mergeCell ref="U31:X31"/>
+    <mergeCell ref="U32:X32"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="H49:L49"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="N27:T27"/>
+    <mergeCell ref="U27:AA27"/>
+    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="N47:Q47"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="U43:X43"/>
+    <mergeCell ref="U44:X44"/>
+    <mergeCell ref="U38:X38"/>
+    <mergeCell ref="U39:X39"/>
+    <mergeCell ref="U40:X40"/>
+    <mergeCell ref="U41:X41"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U34:X34"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U36:X36"/>
+    <mergeCell ref="U37:X37"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="N51:Q51"/>
+    <mergeCell ref="U50:X50"/>
+    <mergeCell ref="U51:X51"/>
+    <mergeCell ref="U45:X45"/>
+    <mergeCell ref="U46:X46"/>
+    <mergeCell ref="U47:X47"/>
+    <mergeCell ref="U48:X48"/>
+    <mergeCell ref="U49:X49"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="N50:Q50"/>
+    <mergeCell ref="N48:Q48"/>
+    <mergeCell ref="N49:Q49"/>
+    <mergeCell ref="N38:Q38"/>
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="N40:Q40"/>
+    <mergeCell ref="N41:Q41"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="N33:Q33"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="U28:X28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="R28:R51">
+  <conditionalFormatting sqref="S28:S51">
     <cfRule type="cellIs" dxfId="14" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R28:R51">
+  <conditionalFormatting sqref="S28:S51">
     <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X28:X51">
+  <conditionalFormatting sqref="Z28:Z51">
     <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X28:X51">
+  <conditionalFormatting sqref="Z28:Z51">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -3565,9 +3713,7 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -3648,7 +3794,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
@@ -3665,7 +3811,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
@@ -3682,7 +3828,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
@@ -3715,7 +3861,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -3731,7 +3877,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -3755,18 +3901,18 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A5" s="19" t="s">
-        <v>32</v>
+      <c r="A5" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="3">
         <v>3344110</v>
@@ -3777,18 +3923,18 @@
       <c r="D5" s="3">
         <v>3334440</v>
       </c>
-      <c r="F5" s="20">
-        <f>$B5/$C5-1</f>
+      <c r="F5" s="19">
+        <f>IF($C5=0,0,$B5/$C5-1)</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G5" s="20">
-        <f>$B5/$D5-1</f>
+      <c r="G5" s="19">
+        <f>IF($D5=0,0,$B5/$D5-1)</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A6" s="19" t="s">
-        <v>33</v>
+      <c r="A6" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="3">
         <v>3323110</v>
@@ -3799,18 +3945,18 @@
       <c r="D6" s="3">
         <v>3323440</v>
       </c>
-      <c r="F6" s="20">
-        <f t="shared" ref="F6:F28" si="0">$B6/$C6-1</f>
+      <c r="F6" s="19">
+        <f t="shared" ref="F6:F28" si="0">IF($C6=0,0,$B6/$C6-1)</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="G6" s="20">
-        <f t="shared" ref="G6:G28" si="1">$B6/$D6-1</f>
+      <c r="G6" s="19">
+        <f t="shared" ref="G6:G28" si="1">IF($D6=0,0,$B6/$D6-1)</f>
         <v>-9.9294706689456724E-5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A7" s="19" t="s">
-        <v>34</v>
+      <c r="A7" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="B7" s="3">
         <v>3344110</v>
@@ -3821,18 +3967,18 @@
       <c r="D7" s="3">
         <v>3324440</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="19">
         <f t="shared" si="1"/>
         <v>5.9167859850079996E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A8" s="19" t="s">
-        <v>35</v>
+      <c r="A8" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="3">
         <v>3344110</v>
@@ -3843,18 +3989,18 @@
       <c r="D8" s="3">
         <v>3334440</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A9" s="19" t="s">
-        <v>36</v>
+      <c r="A9" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="3">
         <v>3344110</v>
@@ -3865,18 +4011,18 @@
       <c r="D9" s="3">
         <v>3244440</v>
       </c>
-      <c r="F9" s="20">
+      <c r="F9" s="19">
         <f t="shared" si="0"/>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="19">
         <f t="shared" si="1"/>
         <v>3.0720247561982994E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A10" s="19" t="s">
-        <v>40</v>
+      <c r="A10" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>3344110</v>
@@ -3887,18 +4033,18 @@
       <c r="D10" s="3">
         <v>3334440</v>
       </c>
-      <c r="F10" s="20">
+      <c r="F10" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A11" s="19" t="s">
-        <v>41</v>
+      <c r="A11" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="B11" s="3">
         <v>4344110</v>
@@ -3909,18 +4055,18 @@
       <c r="D11" s="3">
         <v>3334440</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <f t="shared" si="0"/>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <f t="shared" si="1"/>
         <v>0.30280047024387913</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A12" s="19" t="s">
-        <v>42</v>
+      <c r="A12" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="B12" s="3">
         <v>3344110</v>
@@ -3931,18 +4077,18 @@
       <c r="D12" s="3">
         <v>3554440</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="19">
         <f t="shared" si="1"/>
         <v>-5.9173878304317973E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A13" s="19" t="s">
-        <v>43</v>
+      <c r="A13" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="B13" s="3">
         <v>3344110</v>
@@ -3953,18 +4099,18 @@
       <c r="D13" s="3">
         <v>3674440</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="19">
         <f t="shared" si="1"/>
         <v>-8.9899413243922921E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A14" s="19" t="s">
-        <v>44</v>
+      <c r="A14" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="B14" s="3">
         <v>3344110</v>
@@ -3975,18 +4121,18 @@
       <c r="D14" s="3">
         <v>3334440</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A15" s="19" t="s">
-        <v>45</v>
+      <c r="A15" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="B15" s="3">
         <v>3344110</v>
@@ -3997,18 +4143,18 @@
       <c r="D15" s="3">
         <v>3544440</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="19">
         <f t="shared" si="1"/>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A16" s="19" t="s">
-        <v>46</v>
+      <c r="A16" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B16" s="3">
         <v>3344110</v>
@@ -4019,18 +4165,18 @@
       <c r="D16" s="3">
         <v>3334440</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A17" s="19" t="s">
-        <v>47</v>
+      <c r="A17" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="B17" s="3">
         <v>3344110</v>
@@ -4041,18 +4187,18 @@
       <c r="D17" s="3">
         <v>3334440</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A18" s="19" t="s">
-        <v>48</v>
+      <c r="A18" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="B18" s="3">
         <v>3484110</v>
@@ -4063,18 +4209,18 @@
       <c r="D18" s="3">
         <v>3344440</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="19">
         <f t="shared" si="0"/>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="19">
         <f t="shared" si="1"/>
         <v>4.1761849517407912E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A19" s="19" t="s">
-        <v>49</v>
+      <c r="A19" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="B19" s="3">
         <v>3344110</v>
@@ -4085,18 +4231,18 @@
       <c r="D19" s="3">
         <v>3334440</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A20" s="19" t="s">
-        <v>50</v>
+      <c r="A20" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="B20" s="3">
         <v>3344110</v>
@@ -4107,18 +4253,18 @@
       <c r="D20" s="3">
         <v>3544440</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="19">
         <f t="shared" si="1"/>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A21" s="19" t="s">
-        <v>51</v>
+      <c r="A21" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="B21" s="3">
         <v>3344110</v>
@@ -4129,18 +4275,18 @@
       <c r="D21" s="3">
         <v>3334440</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="19">
         <f t="shared" si="0"/>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A22" s="19" t="s">
-        <v>52</v>
+      <c r="A22" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="B22" s="3">
         <v>3344110</v>
@@ -4151,18 +4297,18 @@
       <c r="D22" s="3">
         <v>3334440</v>
       </c>
-      <c r="F22" s="20">
+      <c r="F22" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A23" s="19" t="s">
-        <v>53</v>
+      <c r="A23" s="18" t="s">
+        <v>52</v>
       </c>
       <c r="B23" s="3">
         <v>3344110</v>
@@ -4173,18 +4319,18 @@
       <c r="D23" s="3">
         <v>3334440</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A24" s="19" t="s">
-        <v>54</v>
+      <c r="A24" s="18" t="s">
+        <v>53</v>
       </c>
       <c r="B24" s="3">
         <v>2144110</v>
@@ -4195,18 +4341,18 @@
       <c r="D24" s="3">
         <v>3334440</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="19">
         <f t="shared" si="0"/>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="19">
         <f t="shared" si="1"/>
         <v>-0.35698048247981673</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A25" s="19" t="s">
-        <v>55</v>
+      <c r="A25" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="B25" s="3">
         <v>3344110</v>
@@ -4217,18 +4363,18 @@
       <c r="D25" s="3">
         <v>3334440</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A26" s="19" t="s">
-        <v>56</v>
+      <c r="A26" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="B26" s="3">
         <v>3344110</v>
@@ -4239,18 +4385,18 @@
       <c r="D26" s="3">
         <v>3334440</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G26" s="20">
+      <c r="G26" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A27" s="19" t="s">
-        <v>57</v>
+      <c r="A27" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="B27" s="3">
         <v>3344110</v>
@@ -4261,18 +4407,18 @@
       <c r="D27" s="3">
         <v>3334440</v>
       </c>
-      <c r="F27" s="20">
+      <c r="F27" s="19">
         <f t="shared" si="0"/>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="G27" s="20">
+      <c r="G27" s="19">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A28" s="19" t="s">
-        <v>58</v>
+      <c r="A28" s="18" t="s">
+        <v>57</v>
       </c>
       <c r="B28" s="3">
         <v>3344110</v>
@@ -4283,11 +4429,11 @@
       <c r="D28" s="3">
         <v>3214440</v>
       </c>
-      <c r="F28" s="20">
+      <c r="F28" s="19">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G28" s="20">
+      <c r="G28" s="19">
         <f t="shared" si="1"/>
         <v>4.0339841465387494E-2</v>
       </c>

</xml_diff>

<commit_message>
rill-analysis: Add jdbc data support
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
@@ -416,6 +416,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="177" formatCode="#,##0.0000_ "/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -820,7 +824,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -829,9 +833,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -899,14 +900,11 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -923,13 +921,13 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,10 +936,19 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1242,7 +1249,7 @@
             <c:numRef>
               <c:f>_input!$B$5:$B$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3344110</c:v>
@@ -1418,7 +1425,7 @@
             <c:numRef>
               <c:f>_input!$C$5:$C$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3224110</c:v>
@@ -1594,7 +1601,7 @@
             <c:numRef>
               <c:f>_input!$D$5:$D$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>#,##0.0000</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3334440</c:v>
@@ -1673,11 +1680,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="99315072"/>
-        <c:axId val="99329152"/>
+        <c:axId val="87321600"/>
+        <c:axId val="87343872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99315072"/>
+        <c:axId val="87321600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,23 +1693,23 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99329152"/>
+        <c:crossAx val="87343872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99329152"/>
+        <c:axId val="87343872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99315072"/>
+        <c:crossAx val="87321600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1720,7 +1727,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000081" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000081" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000833" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000833" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1772,7 +1779,7 @@
     <tableColumn id="5" name="依赖关系" dataDxfId="2">
       <calculatedColumnFormula>$B8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="源" dataDxfId="1" dataCellStyle="超链接"/>
+    <tableColumn id="6" name="源" dataDxfId="1"/>
     <tableColumn id="7" name="格式" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2076,1730 +2083,1726 @@
     <col min="13" max="13" width="1.125" customWidth="1"/>
     <col min="14" max="17" width="6.125" customWidth="1"/>
     <col min="18" max="18" width="1.5" customWidth="1"/>
-    <col min="19" max="19" width="8.625" customWidth="1"/>
+    <col min="19" max="19" width="10.125" customWidth="1"/>
     <col min="20" max="20" width="1.5" customWidth="1"/>
     <col min="21" max="21" width="2.375" customWidth="1"/>
     <col min="22" max="25" width="6.125" customWidth="1"/>
     <col min="26" max="26" width="1.5" customWidth="1"/>
-    <col min="27" max="27" width="8.625" customWidth="1"/>
+    <col min="27" max="27" width="10.125" customWidth="1"/>
     <col min="28" max="28" width="1.5" customWidth="1"/>
     <col min="29" max="29" width="2.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="3.75" customHeight="1">
-      <c r="R1" s="5"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" spans="2:18">
-      <c r="B2" s="30" t="str">
+      <c r="B2" s="28" t="str">
         <f>_input!$A2&amp;"+"&amp;_input!$A3&amp;"+趋势图"</f>
         <v>商业产品线+分析指标+趋势图</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="R2" s="5"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" spans="2:18">
-      <c r="R3" s="5"/>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="29" t="str">
+      <c r="B4" s="27" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="R4" s="5"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="2:18" ht="3" customHeight="1">
-      <c r="R5" s="5"/>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="2:18">
-      <c r="R6" s="5"/>
+      <c r="R6" s="4"/>
     </row>
     <row r="7" spans="2:18">
-      <c r="R7" s="5"/>
+      <c r="R7" s="4"/>
     </row>
     <row r="8" spans="2:18">
-      <c r="R8" s="5"/>
+      <c r="R8" s="4"/>
     </row>
     <row r="9" spans="2:18">
-      <c r="R9" s="5"/>
+      <c r="R9" s="4"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="R10" s="5"/>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="R11" s="5"/>
+      <c r="R11" s="4"/>
     </row>
     <row r="12" spans="2:18">
-      <c r="R12" s="5"/>
+      <c r="R12" s="4"/>
     </row>
     <row r="13" spans="2:18">
-      <c r="R13" s="5"/>
+      <c r="R13" s="4"/>
     </row>
     <row r="14" spans="2:18">
-      <c r="R14" s="5"/>
+      <c r="R14" s="4"/>
     </row>
     <row r="15" spans="2:18">
-      <c r="R15" s="5"/>
+      <c r="R15" s="4"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="R16" s="5"/>
+      <c r="R16" s="4"/>
     </row>
     <row r="17" spans="1:29">
-      <c r="R17" s="5"/>
+      <c r="R17" s="4"/>
     </row>
     <row r="18" spans="1:29">
-      <c r="R18" s="5"/>
+      <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="R19" s="5"/>
+      <c r="R19" s="4"/>
     </row>
     <row r="20" spans="1:29">
-      <c r="R20" s="5"/>
+      <c r="R20" s="4"/>
     </row>
     <row r="21" spans="1:29">
-      <c r="R21" s="5"/>
+      <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:29">
-      <c r="R22" s="5"/>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:29">
-      <c r="R23" s="5"/>
+      <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:29">
-      <c r="B24" s="30" t="str">
+      <c r="B24" s="28" t="str">
         <f>_input!$B3&amp;"分小时数据表"</f>
         <v>点击消费分小时数据表</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="R24" s="5"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="R24" s="4"/>
       <c r="X24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="3.75" customHeight="1"/>
     <row r="26" spans="1:29" ht="3" customHeight="1">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="19"/>
-      <c r="X26" s="19"/>
-      <c r="Y26" s="19"/>
-      <c r="Z26" s="19"/>
-      <c r="AA26" s="19"/>
-      <c r="AB26" s="19"/>
-      <c r="AC26" s="19"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
     </row>
     <row r="27" spans="1:29" ht="35.25" customHeight="1">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="37" t="s">
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="26" t="s">
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="28"/>
-      <c r="V27" s="26" t="s">
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="39"/>
+      <c r="V27" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="27"/>
-      <c r="AA27" s="27"/>
-      <c r="AB27" s="27"/>
-      <c r="AC27" s="28"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="38"/>
+      <c r="AC27" s="39"/>
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="41" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="39">
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="40">
         <f>_input!$B5</f>
         <v>3344110</v>
       </c>
-      <c r="I28" s="40"/>
-      <c r="J28" s="40"/>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="34">
-        <f>_input!$C5</f>
-        <v>3224110</v>
-      </c>
-      <c r="O28" s="35"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="20" t="s">
+      <c r="I28" s="41"/>
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="32">
+        <f>_input!$H5</f>
+        <v>120000</v>
+      </c>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S28" s="21">
+      <c r="S28" s="20">
         <f>_input!$F5</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T28" s="20" t="s">
+      <c r="T28" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U28" s="25">
+      <c r="U28" s="24">
         <f>_input!$F5</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V28" s="35">
-        <f>_input!$D5</f>
-        <v>3334440</v>
-      </c>
-      <c r="W28" s="35"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="20" t="s">
+      <c r="V28" s="34">
+        <f>_input!$I5</f>
+        <v>9670</v>
+      </c>
+      <c r="W28" s="34"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA28" s="21">
+      <c r="AA28" s="20">
         <f>_input!$G5</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB28" s="20" t="s">
+      <c r="AB28" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC28" s="25">
+      <c r="AC28" s="24">
         <f>_input!$G5</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="15" customHeight="1">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="41" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="39">
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="40">
         <f>_input!$B6</f>
         <v>3323110</v>
       </c>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="34">
-        <f>_input!$C6</f>
-        <v>4343110</v>
-      </c>
-      <c r="O29" s="35"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="20" t="s">
+      <c r="I29" s="41"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="32">
+        <f>_input!$H6</f>
+        <v>-1020000</v>
+      </c>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S29" s="21">
+      <c r="S29" s="20">
         <f>_input!$F6</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="T29" s="20" t="s">
+      <c r="T29" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U29" s="25">
+      <c r="U29" s="24">
         <f>_input!$F6</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="V29" s="35">
-        <f>_input!$D6</f>
-        <v>3323440</v>
-      </c>
-      <c r="W29" s="35"/>
-      <c r="X29" s="36"/>
-      <c r="Y29" s="36"/>
-      <c r="Z29" s="20" t="s">
+      <c r="V29" s="34">
+        <f>_input!$I6</f>
+        <v>-330</v>
+      </c>
+      <c r="W29" s="34"/>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA29" s="21">
+      <c r="AA29" s="20">
         <f>_input!$G6</f>
         <v>-9.9294706689456724E-5</v>
       </c>
-      <c r="AB29" s="20" t="s">
+      <c r="AB29" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC29" s="25">
+      <c r="AC29" s="24">
         <f>_input!$G6</f>
         <v>-9.9294706689456724E-5</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="15" customHeight="1">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="41" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="39">
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="40">
         <f>_input!$B7</f>
         <v>3344110</v>
       </c>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="34">
-        <f>_input!$C7</f>
-        <v>3224110</v>
-      </c>
-      <c r="O30" s="35"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="20" t="s">
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="32">
+        <f>_input!$H7</f>
+        <v>120000</v>
+      </c>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S30" s="21">
+      <c r="S30" s="20">
         <f>_input!$F7</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T30" s="20" t="s">
+      <c r="T30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U30" s="25">
+      <c r="U30" s="24">
         <f>_input!$F7</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V30" s="35">
-        <f>_input!$D7</f>
-        <v>3324440</v>
-      </c>
-      <c r="W30" s="35"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="20" t="s">
+      <c r="V30" s="34">
+        <f>_input!$I7</f>
+        <v>19670</v>
+      </c>
+      <c r="W30" s="34"/>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA30" s="21">
+      <c r="AA30" s="20">
         <f>_input!$G7</f>
         <v>5.9167859850079996E-3</v>
       </c>
-      <c r="AB30" s="20" t="s">
+      <c r="AB30" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC30" s="25">
+      <c r="AC30" s="24">
         <f>_input!$G7</f>
         <v>5.9167859850079996E-3</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="15" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="41" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="39">
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="40">
         <f>_input!$B8</f>
         <v>3344110</v>
       </c>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="34">
-        <f>_input!$C8</f>
-        <v>3224110</v>
-      </c>
-      <c r="O31" s="35"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="20" t="s">
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="32">
+        <f>_input!$H8</f>
+        <v>120000</v>
+      </c>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S31" s="21">
+      <c r="S31" s="20">
         <f>_input!$F8</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T31" s="20" t="s">
+      <c r="T31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U31" s="25">
+      <c r="U31" s="24">
         <f>_input!$F8</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V31" s="35">
-        <f>_input!$D8</f>
-        <v>3334440</v>
-      </c>
-      <c r="W31" s="35"/>
-      <c r="X31" s="36"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="20" t="s">
+      <c r="V31" s="34">
+        <f>_input!$I8</f>
+        <v>9670</v>
+      </c>
+      <c r="W31" s="34"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="34"/>
+      <c r="Z31" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA31" s="21">
+      <c r="AA31" s="20">
         <f>_input!$G8</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB31" s="20" t="s">
+      <c r="AB31" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC31" s="25">
+      <c r="AC31" s="24">
         <f>_input!$G8</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="15" customHeight="1">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="41" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="39">
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="40">
         <f>_input!$B9</f>
         <v>3344110</v>
       </c>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="34">
-        <f>_input!$C9</f>
-        <v>3664110</v>
-      </c>
-      <c r="O32" s="35"/>
-      <c r="P32" s="36"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="20" t="s">
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="32">
+        <f>_input!$H9</f>
+        <v>-320000</v>
+      </c>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S32" s="21">
+      <c r="S32" s="20">
         <f>_input!$F9</f>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="T32" s="20" t="s">
+      <c r="T32" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U32" s="25">
+      <c r="U32" s="24">
         <f>_input!$F9</f>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="V32" s="35">
-        <f>_input!$D9</f>
-        <v>3244440</v>
-      </c>
-      <c r="W32" s="35"/>
-      <c r="X32" s="36"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="20" t="s">
+      <c r="V32" s="34">
+        <f>_input!$I9</f>
+        <v>99670</v>
+      </c>
+      <c r="W32" s="34"/>
+      <c r="X32" s="34"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA32" s="21">
+      <c r="AA32" s="20">
         <f>_input!$G9</f>
         <v>3.0720247561982994E-2</v>
       </c>
-      <c r="AB32" s="20" t="s">
+      <c r="AB32" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC32" s="25">
+      <c r="AC32" s="24">
         <f>_input!$G9</f>
         <v>3.0720247561982994E-2</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="15" customHeight="1">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="41" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="39">
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="40">
         <f>_input!$B10</f>
         <v>3344110</v>
       </c>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="40"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="34">
-        <f>_input!$C10</f>
-        <v>3224110</v>
-      </c>
-      <c r="O33" s="35"/>
-      <c r="P33" s="36"/>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="20" t="s">
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="32">
+        <f>_input!$H10</f>
+        <v>120000</v>
+      </c>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S33" s="21">
+      <c r="S33" s="20">
         <f>_input!$F10</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T33" s="20" t="s">
+      <c r="T33" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U33" s="25">
+      <c r="U33" s="24">
         <f>_input!$F10</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V33" s="35">
-        <f>_input!$D10</f>
-        <v>3334440</v>
-      </c>
-      <c r="W33" s="35"/>
-      <c r="X33" s="36"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="20" t="s">
+      <c r="V33" s="34">
+        <f>_input!$I10</f>
+        <v>9670</v>
+      </c>
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA33" s="21">
+      <c r="AA33" s="20">
         <f>_input!$G10</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB33" s="20" t="s">
+      <c r="AB33" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC33" s="25">
+      <c r="AC33" s="24">
         <f>_input!$G10</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="15" customHeight="1">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="41" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="39">
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="40">
         <f>_input!$B11</f>
         <v>4344110</v>
       </c>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="34">
-        <f>_input!$C11</f>
-        <v>4324110</v>
-      </c>
-      <c r="O34" s="35"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="20" t="s">
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="32">
+        <f>_input!$H11</f>
+        <v>20000</v>
+      </c>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S34" s="21">
+      <c r="S34" s="20">
         <f>_input!$F11</f>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="T34" s="20" t="s">
+      <c r="T34" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U34" s="25">
+      <c r="U34" s="24">
         <f>_input!$F11</f>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="V34" s="35">
-        <f>_input!$D11</f>
-        <v>3334440</v>
-      </c>
-      <c r="W34" s="35"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="20" t="s">
+      <c r="V34" s="34">
+        <f>_input!$I11</f>
+        <v>1009670</v>
+      </c>
+      <c r="W34" s="34"/>
+      <c r="X34" s="34"/>
+      <c r="Y34" s="34"/>
+      <c r="Z34" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA34" s="21">
+      <c r="AA34" s="20">
         <f>_input!$G11</f>
         <v>0.30280047024387913</v>
       </c>
-      <c r="AB34" s="20" t="s">
+      <c r="AB34" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC34" s="25">
+      <c r="AC34" s="24">
         <f>_input!$G11</f>
         <v>0.30280047024387913</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="15" customHeight="1">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="41" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="39">
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="40">
         <f>_input!$B12</f>
         <v>3344110</v>
       </c>
-      <c r="I35" s="40"/>
-      <c r="J35" s="40"/>
-      <c r="K35" s="40"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="34">
-        <f>_input!$C12</f>
-        <v>3224110</v>
-      </c>
-      <c r="O35" s="35"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="20" t="s">
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="32">
+        <f>_input!$H12</f>
+        <v>120000</v>
+      </c>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S35" s="21">
+      <c r="S35" s="20">
         <f>_input!$F12</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T35" s="20" t="s">
+      <c r="T35" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U35" s="25">
+      <c r="U35" s="24">
         <f>_input!$F12</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V35" s="35">
-        <f>_input!$D12</f>
-        <v>3554440</v>
-      </c>
-      <c r="W35" s="35"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="36"/>
-      <c r="Z35" s="20" t="s">
+      <c r="V35" s="34">
+        <f>_input!$I12</f>
+        <v>-210330</v>
+      </c>
+      <c r="W35" s="34"/>
+      <c r="X35" s="34"/>
+      <c r="Y35" s="34"/>
+      <c r="Z35" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA35" s="21">
+      <c r="AA35" s="20">
         <f>_input!$G12</f>
         <v>-5.9173878304317973E-2</v>
       </c>
-      <c r="AB35" s="20" t="s">
+      <c r="AB35" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC35" s="25">
+      <c r="AC35" s="24">
         <f>_input!$G12</f>
         <v>-5.9173878304317973E-2</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="15" customHeight="1">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="41" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="39">
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="40">
         <f>_input!$B13</f>
         <v>3344110</v>
       </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-      <c r="K36" s="40"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="34">
-        <f>_input!$C13</f>
-        <v>3224110</v>
-      </c>
-      <c r="O36" s="35"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="20" t="s">
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="32">
+        <f>_input!$H13</f>
+        <v>120000</v>
+      </c>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S36" s="21">
+      <c r="S36" s="20">
         <f>_input!$F13</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T36" s="20" t="s">
+      <c r="T36" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U36" s="25">
+      <c r="U36" s="24">
         <f>_input!$F13</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V36" s="35">
-        <f>_input!$D13</f>
-        <v>3674440</v>
-      </c>
-      <c r="W36" s="35"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="36"/>
-      <c r="Z36" s="20" t="s">
+      <c r="V36" s="34">
+        <f>_input!$I13</f>
+        <v>-330330</v>
+      </c>
+      <c r="W36" s="34"/>
+      <c r="X36" s="34"/>
+      <c r="Y36" s="34"/>
+      <c r="Z36" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA36" s="21">
+      <c r="AA36" s="20">
         <f>_input!$G13</f>
         <v>-8.9899413243922921E-2</v>
       </c>
-      <c r="AB36" s="20" t="s">
+      <c r="AB36" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC36" s="25">
+      <c r="AC36" s="24">
         <f>_input!$G13</f>
         <v>-8.9899413243922921E-2</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="15" customHeight="1">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="41" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="39">
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="40">
         <f>_input!$B14</f>
         <v>3344110</v>
       </c>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="34">
-        <f>_input!$C14</f>
-        <v>3224110</v>
-      </c>
-      <c r="O37" s="35"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="20" t="s">
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="41"/>
+      <c r="L37" s="41"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="32">
+        <f>_input!$H14</f>
+        <v>120000</v>
+      </c>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S37" s="21">
+      <c r="S37" s="20">
         <f>_input!$F14</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T37" s="20" t="s">
+      <c r="T37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U37" s="25">
+      <c r="U37" s="24">
         <f>_input!$F14</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V37" s="35">
-        <f>_input!$D14</f>
-        <v>3334440</v>
-      </c>
-      <c r="W37" s="35"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="20" t="s">
+      <c r="V37" s="34">
+        <f>_input!$I14</f>
+        <v>9670</v>
+      </c>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA37" s="21">
+      <c r="AA37" s="20">
         <f>_input!$G14</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB37" s="20" t="s">
+      <c r="AB37" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC37" s="25">
+      <c r="AC37" s="24">
         <f>_input!$G14</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="15" customHeight="1">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="41" t="s">
+      <c r="B38" s="22"/>
+      <c r="C38" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="39">
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="40">
         <f>_input!$B15</f>
         <v>3344110</v>
       </c>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="34">
-        <f>_input!$C15</f>
-        <v>3524110</v>
-      </c>
-      <c r="O38" s="35"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="20" t="s">
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="32">
+        <f>_input!$H15</f>
+        <v>-180000</v>
+      </c>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S38" s="21">
+      <c r="S38" s="20">
         <f>_input!$F15</f>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="T38" s="20" t="s">
+      <c r="T38" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U38" s="25">
+      <c r="U38" s="24">
         <f>_input!$F15</f>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="V38" s="35">
-        <f>_input!$D15</f>
-        <v>3544440</v>
-      </c>
-      <c r="W38" s="35"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="20" t="s">
+      <c r="V38" s="34">
+        <f>_input!$I15</f>
+        <v>-200330</v>
+      </c>
+      <c r="W38" s="34"/>
+      <c r="X38" s="34"/>
+      <c r="Y38" s="34"/>
+      <c r="Z38" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA38" s="21">
+      <c r="AA38" s="20">
         <f>_input!$G15</f>
         <v>-5.65195066075318E-2</v>
       </c>
-      <c r="AB38" s="20" t="s">
+      <c r="AB38" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC38" s="25">
+      <c r="AC38" s="24">
         <f>_input!$G15</f>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="15" customHeight="1">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="41" t="s">
+      <c r="B39" s="22"/>
+      <c r="C39" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="39">
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="40">
         <f>_input!$B16</f>
         <v>3344110</v>
       </c>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="34">
-        <f>_input!$C16</f>
-        <v>3224110</v>
-      </c>
-      <c r="O39" s="35"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="20" t="s">
+      <c r="I39" s="41"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="41"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="32">
+        <f>_input!$H16</f>
+        <v>120000</v>
+      </c>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S39" s="21">
+      <c r="S39" s="20">
         <f>_input!$F16</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T39" s="20" t="s">
+      <c r="T39" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U39" s="25">
+      <c r="U39" s="24">
         <f>_input!$F16</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V39" s="35">
-        <f>_input!$D16</f>
-        <v>3334440</v>
-      </c>
-      <c r="W39" s="35"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="20" t="s">
+      <c r="V39" s="34">
+        <f>_input!$I16</f>
+        <v>9670</v>
+      </c>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA39" s="21">
+      <c r="AA39" s="20">
         <f>_input!$G16</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB39" s="20" t="s">
+      <c r="AB39" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC39" s="25">
+      <c r="AC39" s="24">
         <f>_input!$G16</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="15" customHeight="1">
-      <c r="A40" s="24" t="s">
+      <c r="A40" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="41" t="s">
+      <c r="B40" s="22"/>
+      <c r="C40" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="39">
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="40">
         <f>_input!$B17</f>
         <v>3344110</v>
       </c>
-      <c r="I40" s="40"/>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="34">
-        <f>_input!$C17</f>
-        <v>3224110</v>
-      </c>
-      <c r="O40" s="35"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="20" t="s">
+      <c r="I40" s="41"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="41"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="32">
+        <f>_input!$H17</f>
+        <v>120000</v>
+      </c>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S40" s="21">
+      <c r="S40" s="20">
         <f>_input!$F17</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T40" s="20" t="s">
+      <c r="T40" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U40" s="25">
+      <c r="U40" s="24">
         <f>_input!$F17</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V40" s="35">
-        <f>_input!$D17</f>
-        <v>3334440</v>
-      </c>
-      <c r="W40" s="35"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="36"/>
-      <c r="Z40" s="20" t="s">
+      <c r="V40" s="34">
+        <f>_input!$I17</f>
+        <v>9670</v>
+      </c>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
+      <c r="Y40" s="34"/>
+      <c r="Z40" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA40" s="21">
+      <c r="AA40" s="20">
         <f>_input!$G17</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB40" s="20" t="s">
+      <c r="AB40" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC40" s="25">
+      <c r="AC40" s="24">
         <f>_input!$G17</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="15" customHeight="1">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="41" t="s">
+      <c r="B41" s="22"/>
+      <c r="C41" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="39">
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="40">
         <f>_input!$B18</f>
         <v>3484110</v>
       </c>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="34">
-        <f>_input!$C18</f>
-        <v>3224110</v>
-      </c>
-      <c r="O41" s="35"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="20" t="s">
+      <c r="I41" s="41"/>
+      <c r="J41" s="41"/>
+      <c r="K41" s="41"/>
+      <c r="L41" s="41"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="32">
+        <f>_input!$H18</f>
+        <v>260000</v>
+      </c>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S41" s="21">
+      <c r="S41" s="20">
         <f>_input!$F18</f>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="T41" s="20" t="s">
+      <c r="T41" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U41" s="25">
+      <c r="U41" s="24">
         <f>_input!$F18</f>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="V41" s="35">
-        <f>_input!$D18</f>
-        <v>3344440</v>
-      </c>
-      <c r="W41" s="35"/>
-      <c r="X41" s="36"/>
-      <c r="Y41" s="36"/>
-      <c r="Z41" s="20" t="s">
+      <c r="V41" s="34">
+        <f>_input!$I18</f>
+        <v>139670</v>
+      </c>
+      <c r="W41" s="34"/>
+      <c r="X41" s="34"/>
+      <c r="Y41" s="34"/>
+      <c r="Z41" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA41" s="21">
+      <c r="AA41" s="20">
         <f>_input!$G18</f>
         <v>4.1761849517407912E-2</v>
       </c>
-      <c r="AB41" s="20" t="s">
+      <c r="AB41" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC41" s="25">
+      <c r="AC41" s="24">
         <f>_input!$G18</f>
         <v>4.1761849517407912E-2</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="15" customHeight="1">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="23"/>
-      <c r="C42" s="41" t="s">
+      <c r="B42" s="22"/>
+      <c r="C42" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="39">
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="40">
         <f>_input!$B19</f>
         <v>3344110</v>
       </c>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="34">
-        <f>_input!$C19</f>
-        <v>3224110</v>
-      </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="36"/>
-      <c r="R42" s="20" t="s">
+      <c r="I42" s="41"/>
+      <c r="J42" s="41"/>
+      <c r="K42" s="41"/>
+      <c r="L42" s="41"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="32">
+        <f>_input!$H19</f>
+        <v>120000</v>
+      </c>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S42" s="21">
+      <c r="S42" s="20">
         <f>_input!$F19</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T42" s="20" t="s">
+      <c r="T42" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U42" s="25">
+      <c r="U42" s="24">
         <f>_input!$F19</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V42" s="35">
-        <f>_input!$D19</f>
-        <v>3334440</v>
-      </c>
-      <c r="W42" s="35"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="20" t="s">
+      <c r="V42" s="34">
+        <f>_input!$I19</f>
+        <v>9670</v>
+      </c>
+      <c r="W42" s="34"/>
+      <c r="X42" s="34"/>
+      <c r="Y42" s="34"/>
+      <c r="Z42" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA42" s="21">
+      <c r="AA42" s="20">
         <f>_input!$G19</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB42" s="20" t="s">
+      <c r="AB42" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC42" s="25">
+      <c r="AC42" s="24">
         <f>_input!$G19</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="15" customHeight="1">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="23"/>
-      <c r="C43" s="41" t="s">
+      <c r="B43" s="22"/>
+      <c r="C43" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="39">
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="40">
         <f>_input!$B20</f>
         <v>3344110</v>
       </c>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="34">
-        <f>_input!$C20</f>
-        <v>3224110</v>
-      </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="36"/>
-      <c r="Q43" s="36"/>
-      <c r="R43" s="20" t="s">
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="41"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="32">
+        <f>_input!$H20</f>
+        <v>120000</v>
+      </c>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S43" s="21">
+      <c r="S43" s="20">
         <f>_input!$F20</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T43" s="20" t="s">
+      <c r="T43" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U43" s="25">
+      <c r="U43" s="24">
         <f>_input!$F20</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V43" s="35">
-        <f>_input!$D20</f>
-        <v>3544440</v>
-      </c>
-      <c r="W43" s="35"/>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="20" t="s">
+      <c r="V43" s="34">
+        <f>_input!$I20</f>
+        <v>-200330</v>
+      </c>
+      <c r="W43" s="34"/>
+      <c r="X43" s="34"/>
+      <c r="Y43" s="34"/>
+      <c r="Z43" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA43" s="21">
+      <c r="AA43" s="20">
         <f>_input!$G20</f>
         <v>-5.65195066075318E-2</v>
       </c>
-      <c r="AB43" s="20" t="s">
+      <c r="AB43" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC43" s="25">
+      <c r="AC43" s="24">
         <f>_input!$G20</f>
         <v>-5.65195066075318E-2</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="15" customHeight="1">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="41" t="s">
+      <c r="B44" s="22"/>
+      <c r="C44" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="41"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="39">
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="40">
         <f>_input!$B21</f>
         <v>3344110</v>
       </c>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="34">
-        <f>_input!$C21</f>
-        <v>3434110</v>
-      </c>
-      <c r="O44" s="35"/>
-      <c r="P44" s="36"/>
-      <c r="Q44" s="36"/>
-      <c r="R44" s="20" t="s">
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
+      <c r="K44" s="41"/>
+      <c r="L44" s="41"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="32">
+        <f>_input!$H21</f>
+        <v>-90000</v>
+      </c>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S44" s="21">
+      <c r="S44" s="20">
         <f>_input!$F21</f>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="T44" s="20" t="s">
+      <c r="T44" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U44" s="25">
+      <c r="U44" s="24">
         <f>_input!$F21</f>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="V44" s="35">
-        <f>_input!$D21</f>
-        <v>3334440</v>
-      </c>
-      <c r="W44" s="35"/>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="20" t="s">
+      <c r="V44" s="34">
+        <f>_input!$I21</f>
+        <v>9670</v>
+      </c>
+      <c r="W44" s="34"/>
+      <c r="X44" s="34"/>
+      <c r="Y44" s="34"/>
+      <c r="Z44" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA44" s="21">
+      <c r="AA44" s="20">
         <f>_input!$G21</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB44" s="20" t="s">
+      <c r="AB44" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC44" s="25">
+      <c r="AC44" s="24">
         <f>_input!$G21</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="15" customHeight="1">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="41" t="s">
+      <c r="B45" s="22"/>
+      <c r="C45" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="39">
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="40">
         <f>_input!$B22</f>
         <v>3344110</v>
       </c>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="40"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="34">
-        <f>_input!$C22</f>
-        <v>3224110</v>
-      </c>
-      <c r="O45" s="35"/>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="36"/>
-      <c r="R45" s="20" t="s">
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="32">
+        <f>_input!$H22</f>
+        <v>120000</v>
+      </c>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
+      <c r="R45" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S45" s="21">
+      <c r="S45" s="20">
         <f>_input!$F22</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T45" s="20" t="s">
+      <c r="T45" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U45" s="25">
+      <c r="U45" s="24">
         <f>_input!$F22</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V45" s="35">
-        <f>_input!$D22</f>
-        <v>3334440</v>
-      </c>
-      <c r="W45" s="35"/>
-      <c r="X45" s="36"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="20" t="s">
+      <c r="V45" s="34">
+        <f>_input!$I22</f>
+        <v>9670</v>
+      </c>
+      <c r="W45" s="34"/>
+      <c r="X45" s="34"/>
+      <c r="Y45" s="34"/>
+      <c r="Z45" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA45" s="21">
+      <c r="AA45" s="20">
         <f>_input!$G22</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB45" s="20" t="s">
+      <c r="AB45" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC45" s="25">
+      <c r="AC45" s="24">
         <f>_input!$G22</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="15" customHeight="1">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="41" t="s">
+      <c r="B46" s="22"/>
+      <c r="C46" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="39">
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="40">
         <f>_input!$B23</f>
         <v>3344110</v>
       </c>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
-      <c r="K46" s="40"/>
-      <c r="L46" s="40"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="34">
-        <f>_input!$C23</f>
-        <v>3224110</v>
-      </c>
-      <c r="O46" s="35"/>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="36"/>
-      <c r="R46" s="20" t="s">
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="32">
+        <f>_input!$H23</f>
+        <v>120000</v>
+      </c>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
+      <c r="R46" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S46" s="21">
+      <c r="S46" s="20">
         <f>_input!$F23</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T46" s="20" t="s">
+      <c r="T46" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U46" s="25">
+      <c r="U46" s="24">
         <f>_input!$F23</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V46" s="35">
-        <f>_input!$D23</f>
-        <v>3334440</v>
-      </c>
-      <c r="W46" s="35"/>
-      <c r="X46" s="36"/>
-      <c r="Y46" s="36"/>
-      <c r="Z46" s="20" t="s">
+      <c r="V46" s="34">
+        <f>_input!$I23</f>
+        <v>9670</v>
+      </c>
+      <c r="W46" s="34"/>
+      <c r="X46" s="34"/>
+      <c r="Y46" s="34"/>
+      <c r="Z46" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA46" s="21">
+      <c r="AA46" s="20">
         <f>_input!$G23</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB46" s="20" t="s">
+      <c r="AB46" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC46" s="25">
+      <c r="AC46" s="24">
         <f>_input!$G23</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="15" customHeight="1">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="41" t="s">
+      <c r="B47" s="22"/>
+      <c r="C47" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="39">
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="40">
         <f>_input!$B24</f>
         <v>2144110</v>
       </c>
-      <c r="I47" s="40"/>
-      <c r="J47" s="40"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="40"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="34">
-        <f>_input!$C24</f>
-        <v>3224110</v>
-      </c>
-      <c r="O47" s="35"/>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="36"/>
-      <c r="R47" s="20" t="s">
+      <c r="I47" s="41"/>
+      <c r="J47" s="41"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="41"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="32">
+        <f>_input!$H24</f>
+        <v>-1080000</v>
+      </c>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S47" s="21">
+      <c r="S47" s="20">
         <f>_input!$F24</f>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="T47" s="20" t="s">
+      <c r="T47" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U47" s="25">
+      <c r="U47" s="24">
         <f>_input!$F24</f>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="V47" s="35">
-        <f>_input!$D24</f>
-        <v>3334440</v>
-      </c>
-      <c r="W47" s="35"/>
-      <c r="X47" s="36"/>
-      <c r="Y47" s="36"/>
-      <c r="Z47" s="20" t="s">
+      <c r="V47" s="34">
+        <f>_input!$I24</f>
+        <v>-1190330</v>
+      </c>
+      <c r="W47" s="34"/>
+      <c r="X47" s="34"/>
+      <c r="Y47" s="34"/>
+      <c r="Z47" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA47" s="21">
+      <c r="AA47" s="20">
         <f>_input!$G24</f>
         <v>-0.35698048247981673</v>
       </c>
-      <c r="AB47" s="20" t="s">
+      <c r="AB47" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC47" s="25">
+      <c r="AC47" s="24">
         <f>_input!$G24</f>
         <v>-0.35698048247981673</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="15" customHeight="1">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="41" t="s">
+      <c r="B48" s="22"/>
+      <c r="C48" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="39">
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="40">
         <f>_input!$B25</f>
         <v>3344110</v>
       </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="34">
-        <f>_input!$C25</f>
-        <v>3224110</v>
-      </c>
-      <c r="O48" s="35"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="36"/>
-      <c r="R48" s="20" t="s">
+      <c r="I48" s="41"/>
+      <c r="J48" s="41"/>
+      <c r="K48" s="41"/>
+      <c r="L48" s="41"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="32">
+        <f>_input!$H25</f>
+        <v>120000</v>
+      </c>
+      <c r="O48" s="33"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S48" s="21">
+      <c r="S48" s="20">
         <f>_input!$F25</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T48" s="20" t="s">
+      <c r="T48" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U48" s="25">
+      <c r="U48" s="24">
         <f>_input!$F25</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V48" s="35">
-        <f>_input!$D25</f>
-        <v>3334440</v>
-      </c>
-      <c r="W48" s="35"/>
-      <c r="X48" s="36"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="20" t="s">
+      <c r="V48" s="34">
+        <f>_input!$I25</f>
+        <v>9670</v>
+      </c>
+      <c r="W48" s="34"/>
+      <c r="X48" s="34"/>
+      <c r="Y48" s="34"/>
+      <c r="Z48" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA48" s="21">
+      <c r="AA48" s="20">
         <f>_input!$G25</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB48" s="20" t="s">
+      <c r="AB48" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC48" s="25">
+      <c r="AC48" s="24">
         <f>_input!$G25</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="15" customHeight="1">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="41" t="s">
+      <c r="B49" s="22"/>
+      <c r="C49" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="39">
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="40">
         <f>_input!$B26</f>
         <v>3344110</v>
       </c>
-      <c r="I49" s="40"/>
-      <c r="J49" s="40"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="40"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="34">
-        <f>_input!$C26</f>
-        <v>3224110</v>
-      </c>
-      <c r="O49" s="35"/>
-      <c r="P49" s="36"/>
-      <c r="Q49" s="36"/>
-      <c r="R49" s="20" t="s">
+      <c r="I49" s="41"/>
+      <c r="J49" s="41"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="41"/>
+      <c r="M49" s="21"/>
+      <c r="N49" s="32">
+        <f>_input!$H26</f>
+        <v>120000</v>
+      </c>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S49" s="21">
+      <c r="S49" s="20">
         <f>_input!$F26</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T49" s="20" t="s">
+      <c r="T49" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U49" s="25">
+      <c r="U49" s="24">
         <f>_input!$F26</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V49" s="35">
-        <f>_input!$D26</f>
-        <v>3334440</v>
-      </c>
-      <c r="W49" s="35"/>
-      <c r="X49" s="36"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="20" t="s">
+      <c r="V49" s="34">
+        <f>_input!$I26</f>
+        <v>9670</v>
+      </c>
+      <c r="W49" s="34"/>
+      <c r="X49" s="34"/>
+      <c r="Y49" s="34"/>
+      <c r="Z49" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA49" s="21">
+      <c r="AA49" s="20">
         <f>_input!$G26</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB49" s="20" t="s">
+      <c r="AB49" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC49" s="25">
+      <c r="AC49" s="24">
         <f>_input!$G26</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="15" customHeight="1">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="41" t="s">
+      <c r="B50" s="22"/>
+      <c r="C50" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="39">
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="40">
         <f>_input!$B27</f>
         <v>3344110</v>
       </c>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
-      <c r="K50" s="40"/>
-      <c r="L50" s="40"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="34">
-        <f>_input!$C27</f>
-        <v>3994110</v>
-      </c>
-      <c r="O50" s="35"/>
-      <c r="P50" s="36"/>
-      <c r="Q50" s="36"/>
-      <c r="R50" s="20" t="s">
+      <c r="I50" s="41"/>
+      <c r="J50" s="41"/>
+      <c r="K50" s="41"/>
+      <c r="L50" s="41"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="32">
+        <f>_input!$H27</f>
+        <v>-650000</v>
+      </c>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S50" s="21">
+      <c r="S50" s="20">
         <f>_input!$F27</f>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="T50" s="20" t="s">
+      <c r="T50" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U50" s="25">
+      <c r="U50" s="24">
         <f>_input!$F27</f>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="V50" s="35">
-        <f>_input!$D27</f>
-        <v>3334440</v>
-      </c>
-      <c r="W50" s="35"/>
-      <c r="X50" s="36"/>
-      <c r="Y50" s="36"/>
-      <c r="Z50" s="20" t="s">
+      <c r="V50" s="34">
+        <f>_input!$I27</f>
+        <v>9670</v>
+      </c>
+      <c r="W50" s="34"/>
+      <c r="X50" s="34"/>
+      <c r="Y50" s="34"/>
+      <c r="Z50" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA50" s="21">
+      <c r="AA50" s="20">
         <f>_input!$G27</f>
         <v>2.9000371876537478E-3</v>
       </c>
-      <c r="AB50" s="20" t="s">
+      <c r="AB50" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC50" s="25">
+      <c r="AC50" s="24">
         <f>_input!$G27</f>
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="15" customHeight="1">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="41" t="s">
+      <c r="B51" s="22"/>
+      <c r="C51" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="39">
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="40">
         <f>_input!$B28</f>
         <v>3344110</v>
       </c>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="34">
-        <f>_input!$C28</f>
-        <v>3224110</v>
-      </c>
-      <c r="O51" s="35"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="36"/>
-      <c r="R51" s="20" t="s">
+      <c r="I51" s="41"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="21"/>
+      <c r="N51" s="32">
+        <f>_input!$H28</f>
+        <v>120000</v>
+      </c>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="S51" s="21">
+      <c r="S51" s="20">
         <f>_input!$F28</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="T51" s="20" t="s">
+      <c r="T51" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="U51" s="25">
+      <c r="U51" s="24">
         <f>_input!$F28</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="V51" s="35">
-        <f>_input!$D28</f>
-        <v>3214440</v>
-      </c>
-      <c r="W51" s="35"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="20" t="s">
+      <c r="V51" s="34">
+        <f>_input!$I28</f>
+        <v>129670</v>
+      </c>
+      <c r="W51" s="34"/>
+      <c r="X51" s="34"/>
+      <c r="Y51" s="34"/>
+      <c r="Z51" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="AA51" s="21">
+      <c r="AA51" s="20">
         <f>_input!$G28</f>
         <v>4.0339841465387494E-2</v>
       </c>
-      <c r="AB51" s="20" t="s">
+      <c r="AB51" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AC51" s="25">
+      <c r="AC51" s="24">
         <f>_input!$G28</f>
         <v>4.0339841465387494E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="C50:G50"/>
     <mergeCell ref="C51:G51"/>
     <mergeCell ref="H50:L50"/>
@@ -3820,7 +3823,6 @@
     <mergeCell ref="C41:G41"/>
     <mergeCell ref="C42:G42"/>
     <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C48:G48"/>
     <mergeCell ref="C49:G49"/>
     <mergeCell ref="H38:L38"/>
     <mergeCell ref="H39:L39"/>
@@ -3838,12 +3840,6 @@
     <mergeCell ref="C45:G45"/>
     <mergeCell ref="C46:G46"/>
     <mergeCell ref="C47:G47"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="H34:L34"/>
     <mergeCell ref="H35:L35"/>
     <mergeCell ref="H36:L36"/>
     <mergeCell ref="V30:Y30"/>
@@ -3852,7 +3848,20 @@
     <mergeCell ref="N35:Q35"/>
     <mergeCell ref="N36:Q36"/>
     <mergeCell ref="V29:Y29"/>
-    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="N27:U27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="V27:AC27"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H34:L34"/>
     <mergeCell ref="N46:Q46"/>
     <mergeCell ref="N47:Q47"/>
     <mergeCell ref="N28:Q28"/>
@@ -3873,9 +3882,6 @@
     <mergeCell ref="V36:Y36"/>
     <mergeCell ref="V37:Y37"/>
     <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="N27:U27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="V27:AC27"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B24:I24"/>
@@ -3899,6 +3905,7 @@
     <mergeCell ref="N42:Q42"/>
     <mergeCell ref="N33:Q33"/>
     <mergeCell ref="V28:Y28"/>
+    <mergeCell ref="H27:M27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="U28:U51">
@@ -3953,79 +3960,79 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14" t="b">
+      <c r="B4" s="13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="27">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -4035,14 +4042,14 @@
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="27">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -4052,11 +4059,11 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="8"/>
+      <c r="G11" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4074,28 +4081,29 @@
   <sheetPr codeName="Sheet3">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="13.75" customWidth="1"/>
     <col min="5" max="5" width="9.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.25" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="9.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1">
+    <row r="1" spans="1:9" ht="18" customHeight="1">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18" customHeight="1">
+    <row r="2" spans="1:9" ht="18" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -4103,7 +4111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18" customHeight="1">
+    <row r="3" spans="1:9" ht="18" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -4111,7 +4119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" thickBot="1">
+    <row r="4" spans="1:9" ht="14.25" thickBot="1">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -4125,532 +4133,724 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="25">
         <v>3344110</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="25">
         <v>3224110</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="25">
         <v>3334440</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <f>IF($C5=0,0,$B5/$C5-1)</f>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <f>IF($D5=0,0,$B5/$D5-1)</f>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A6" s="17" t="s">
+      <c r="H5" s="26">
+        <f>$B5-$C5</f>
+        <v>120000</v>
+      </c>
+      <c r="I5" s="26">
+        <f>$B5-$D5</f>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="25">
         <v>3323110</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="25">
         <v>4343110</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="25">
         <v>3323440</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <f t="shared" ref="F6:F28" si="0">IF($C6=0,0,$B6/$C6-1)</f>
         <v>-0.23485474694401021</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <f t="shared" ref="G6:G28" si="1">IF($D6=0,0,$B6/$D6-1)</f>
         <v>-9.9294706689456724E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A7" s="17" t="s">
+      <c r="H6" s="26">
+        <f t="shared" ref="H6:H28" si="2">$B6-$C6</f>
+        <v>-1020000</v>
+      </c>
+      <c r="I6" s="26">
+        <f t="shared" ref="I6:I28" si="3">$B6-$D6</f>
+        <v>-330</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="25">
         <v>3344110</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="25">
         <v>3224110</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="25">
         <v>3324440</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <f t="shared" si="1"/>
         <v>5.9167859850079996E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A8" s="17" t="s">
+      <c r="H7" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I7" s="26">
+        <f t="shared" si="3"/>
+        <v>19670</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="25">
         <v>3344110</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="25">
         <v>3224110</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="25">
         <v>3334440</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A9" s="17" t="s">
+      <c r="H8" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I8" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A9" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="25">
         <v>3344110</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="25">
         <v>3664110</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="25">
         <v>3244440</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <f t="shared" si="0"/>
         <v>-8.7333622625958229E-2</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <f t="shared" si="1"/>
         <v>3.0720247561982994E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A10" s="17" t="s">
+      <c r="H9" s="26">
+        <f t="shared" si="2"/>
+        <v>-320000</v>
+      </c>
+      <c r="I9" s="26">
+        <f t="shared" si="3"/>
+        <v>99670</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="25">
         <v>3344110</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="25">
         <v>3224110</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="25">
         <v>3334440</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A11" s="17" t="s">
+      <c r="H10" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I10" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A11" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="25">
         <v>4344110</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="25">
         <v>4324110</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="25">
         <v>3334440</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f t="shared" si="0"/>
         <v>4.6252292379240778E-3</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <f t="shared" si="1"/>
         <v>0.30280047024387913</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A12" s="17" t="s">
+      <c r="H11" s="26">
+        <f t="shared" si="2"/>
+        <v>20000</v>
+      </c>
+      <c r="I11" s="26">
+        <f t="shared" si="3"/>
+        <v>1009670</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="25">
         <v>3344110</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="25">
         <v>3224110</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="25">
         <v>3554440</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <f t="shared" si="1"/>
         <v>-5.9173878304317973E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A13" s="17" t="s">
+      <c r="H12" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I12" s="26">
+        <f t="shared" si="3"/>
+        <v>-210330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A13" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="25">
         <v>3344110</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="25">
         <v>3224110</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="25">
         <v>3674440</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <f t="shared" si="1"/>
         <v>-8.9899413243922921E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A14" s="17" t="s">
+      <c r="H13" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I13" s="26">
+        <f t="shared" si="3"/>
+        <v>-330330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A14" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="25">
         <v>3344110</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="25">
         <v>3224110</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="25">
         <v>3334440</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A15" s="17" t="s">
+      <c r="H14" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I14" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="25">
         <v>3344110</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="25">
         <v>3524110</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="25">
         <v>3544440</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <f t="shared" si="0"/>
         <v>-5.1076725754871433E-2</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="17">
         <f t="shared" si="1"/>
         <v>-5.65195066075318E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A16" s="17" t="s">
+      <c r="H15" s="26">
+        <f t="shared" si="2"/>
+        <v>-180000</v>
+      </c>
+      <c r="I15" s="26">
+        <f t="shared" si="3"/>
+        <v>-200330</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="25">
         <v>3344110</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="25">
         <v>3224110</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="25">
         <v>3334440</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A17" s="17" t="s">
+      <c r="H16" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I16" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A17" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="25">
         <v>3344110</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="25">
         <v>3224110</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="25">
         <v>3334440</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A18" s="17" t="s">
+      <c r="H17" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I17" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A18" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="25">
         <v>3484110</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="25">
         <v>3224110</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="25">
         <v>3344440</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <f t="shared" si="0"/>
         <v>8.0642409843336704E-2</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="17">
         <f t="shared" si="1"/>
         <v>4.1761849517407912E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A19" s="17" t="s">
+      <c r="H18" s="26">
+        <f t="shared" si="2"/>
+        <v>260000</v>
+      </c>
+      <c r="I18" s="26">
+        <f t="shared" si="3"/>
+        <v>139670</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="25">
         <v>3344110</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="25">
         <v>3224110</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="25">
         <v>3334440</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A20" s="17" t="s">
+      <c r="H19" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I19" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="25">
         <v>3344110</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="25">
         <v>3224110</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="25">
         <v>3544440</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="17">
         <f t="shared" si="1"/>
         <v>-5.65195066075318E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A21" s="17" t="s">
+      <c r="H20" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I20" s="26">
+        <f t="shared" si="3"/>
+        <v>-200330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="25">
         <v>3344110</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="25">
         <v>3434110</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="25">
         <v>3334440</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <f t="shared" si="0"/>
         <v>-2.6207663703259332E-2</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A22" s="17" t="s">
+      <c r="H21" s="26">
+        <f t="shared" si="2"/>
+        <v>-90000</v>
+      </c>
+      <c r="I21" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A22" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="25">
         <v>3344110</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="25">
         <v>3224110</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="25">
         <v>3334440</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A23" s="17" t="s">
+      <c r="H22" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I22" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A23" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="25">
         <v>3344110</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="25">
         <v>3224110</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="25">
         <v>3334440</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G23" s="18">
+      <c r="G23" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A24" s="17" t="s">
+      <c r="H23" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I23" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A24" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="25">
         <v>2144110</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="25">
         <v>3224110</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="25">
         <v>3334440</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="17">
         <f t="shared" si="0"/>
         <v>-0.33497616396462904</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="17">
         <f t="shared" si="1"/>
         <v>-0.35698048247981673</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A25" s="17" t="s">
+      <c r="H24" s="26">
+        <f t="shared" si="2"/>
+        <v>-1080000</v>
+      </c>
+      <c r="I24" s="26">
+        <f t="shared" si="3"/>
+        <v>-1190330</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A25" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="25">
         <v>3344110</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="25">
         <v>3224110</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="25">
         <v>3334440</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A26" s="17" t="s">
+      <c r="H25" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I25" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A26" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="25">
         <v>3344110</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="25">
         <v>3224110</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="25">
         <v>3334440</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A27" s="17" t="s">
+      <c r="H26" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I26" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A27" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="25">
         <v>3344110</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="25">
         <v>3994110</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="25">
         <v>3334440</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="17">
         <f t="shared" si="0"/>
         <v>-0.16273963411122883</v>
       </c>
-      <c r="G27" s="18">
+      <c r="G27" s="17">
         <f t="shared" si="1"/>
         <v>2.9000371876537478E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="14.25" thickBot="1">
-      <c r="A28" s="17" t="s">
+      <c r="H27" s="26">
+        <f t="shared" si="2"/>
+        <v>-650000</v>
+      </c>
+      <c r="I27" s="26">
+        <f t="shared" si="3"/>
+        <v>9670</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.25" thickBot="1">
+      <c r="A28" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="25">
         <v>3344110</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="25">
         <v>3224110</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="25">
         <v>3214440</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="17">
         <f t="shared" si="1"/>
         <v>4.0339841465387494E-2</v>
+      </c>
+      <c r="H28" s="26">
+        <f t="shared" si="2"/>
+        <v>120000</v>
+      </c>
+      <c r="I28" s="26">
+        <f t="shared" si="3"/>
+        <v>129670</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rill-analysis: Enhance browser compatible
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="91">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -409,6 +409,10 @@
   </si>
   <si>
     <t>同比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,9 +420,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0000_ "/>
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -900,10 +903,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -921,13 +924,13 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -935,6 +938,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,18 +959,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1249,7 +1252,7 @@
             <c:numRef>
               <c:f>_input!$B$5:$B$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3344110</c:v>
@@ -1425,7 +1428,7 @@
             <c:numRef>
               <c:f>_input!$C$5:$C$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3224110</c:v>
@@ -1601,7 +1604,7 @@
             <c:numRef>
               <c:f>_input!$D$5:$D$28</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>3334440</c:v>
@@ -1680,11 +1683,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87321600"/>
-        <c:axId val="87343872"/>
+        <c:axId val="85748736"/>
+        <c:axId val="85771008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87321600"/>
+        <c:axId val="85748736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,23 +1696,23 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87343872"/>
+        <c:crossAx val="85771008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87343872"/>
+        <c:axId val="85771008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87321600"/>
+        <c:crossAx val="85748736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1727,7 +1730,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000833" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000833" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000855" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000855" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2071,9 +2074,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC51"/>
+  <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="AD52" sqref="AD52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -2244,47 +2249,47 @@
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
       <c r="M27" s="36"/>
-      <c r="N27" s="37" t="s">
+      <c r="N27" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="38"/>
-      <c r="S27" s="38"/>
-      <c r="T27" s="38"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="37" t="s">
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="W27" s="38"/>
-      <c r="X27" s="38"/>
-      <c r="Y27" s="38"/>
-      <c r="Z27" s="38"/>
-      <c r="AA27" s="38"/>
-      <c r="AB27" s="38"/>
-      <c r="AC27" s="39"/>
+      <c r="W27" s="42"/>
+      <c r="X27" s="42"/>
+      <c r="Y27" s="42"/>
+      <c r="Z27" s="42"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="42"/>
+      <c r="AC27" s="43"/>
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1">
       <c r="A28" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B28" s="22"/>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="40">
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="39">
         <f>_input!$B5</f>
         <v>3344110</v>
       </c>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
       <c r="M28" s="21"/>
       <c r="N28" s="32">
         <f>_input!$H5</f>
@@ -2334,21 +2339,21 @@
         <v>88</v>
       </c>
       <c r="B29" s="22"/>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="40">
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="39">
         <f>_input!$B6</f>
         <v>3323110</v>
       </c>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
       <c r="M29" s="21"/>
       <c r="N29" s="32">
         <f>_input!$H6</f>
@@ -2398,21 +2403,21 @@
         <v>88</v>
       </c>
       <c r="B30" s="22"/>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="40">
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="39">
         <f>_input!$B7</f>
         <v>3344110</v>
       </c>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
       <c r="M30" s="21"/>
       <c r="N30" s="32">
         <f>_input!$H7</f>
@@ -2462,21 +2467,21 @@
         <v>88</v>
       </c>
       <c r="B31" s="22"/>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="40">
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="39">
         <f>_input!$B8</f>
         <v>3344110</v>
       </c>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
       <c r="M31" s="21"/>
       <c r="N31" s="32">
         <f>_input!$H8</f>
@@ -2526,21 +2531,21 @@
         <v>88</v>
       </c>
       <c r="B32" s="22"/>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="40">
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="39">
         <f>_input!$B9</f>
         <v>3344110</v>
       </c>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
       <c r="M32" s="21"/>
       <c r="N32" s="32">
         <f>_input!$H9</f>
@@ -2590,21 +2595,21 @@
         <v>88</v>
       </c>
       <c r="B33" s="22"/>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="40">
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="39">
         <f>_input!$B10</f>
         <v>3344110</v>
       </c>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
       <c r="M33" s="21"/>
       <c r="N33" s="32">
         <f>_input!$H10</f>
@@ -2654,21 +2659,21 @@
         <v>88</v>
       </c>
       <c r="B34" s="22"/>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="40">
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="39">
         <f>_input!$B11</f>
         <v>4344110</v>
       </c>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
       <c r="M34" s="21"/>
       <c r="N34" s="32">
         <f>_input!$H11</f>
@@ -2718,21 +2723,21 @@
         <v>88</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="40">
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="39">
         <f>_input!$B12</f>
         <v>3344110</v>
       </c>
-      <c r="I35" s="41"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+      <c r="K35" s="40"/>
+      <c r="L35" s="40"/>
       <c r="M35" s="21"/>
       <c r="N35" s="32">
         <f>_input!$H12</f>
@@ -2782,21 +2787,21 @@
         <v>88</v>
       </c>
       <c r="B36" s="22"/>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="40">
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="39">
         <f>_input!$B13</f>
         <v>3344110</v>
       </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
       <c r="M36" s="21"/>
       <c r="N36" s="32">
         <f>_input!$H13</f>
@@ -2846,21 +2851,21 @@
         <v>88</v>
       </c>
       <c r="B37" s="22"/>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="40">
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="39">
         <f>_input!$B14</f>
         <v>3344110</v>
       </c>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
       <c r="M37" s="21"/>
       <c r="N37" s="32">
         <f>_input!$H14</f>
@@ -2910,21 +2915,21 @@
         <v>88</v>
       </c>
       <c r="B38" s="22"/>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="42"/>
-      <c r="E38" s="42"/>
-      <c r="F38" s="42"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="40">
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="39">
         <f>_input!$B15</f>
         <v>3344110</v>
       </c>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
       <c r="M38" s="21"/>
       <c r="N38" s="32">
         <f>_input!$H15</f>
@@ -2974,21 +2979,21 @@
         <v>88</v>
       </c>
       <c r="B39" s="22"/>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="40">
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="39">
         <f>_input!$B16</f>
         <v>3344110</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
       <c r="M39" s="21"/>
       <c r="N39" s="32">
         <f>_input!$H16</f>
@@ -3038,21 +3043,21 @@
         <v>88</v>
       </c>
       <c r="B40" s="22"/>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="40">
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="39">
         <f>_input!$B17</f>
         <v>3344110</v>
       </c>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
       <c r="M40" s="21"/>
       <c r="N40" s="32">
         <f>_input!$H17</f>
@@ -3102,21 +3107,21 @@
         <v>88</v>
       </c>
       <c r="B41" s="22"/>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="40">
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="39">
         <f>_input!$B18</f>
         <v>3484110</v>
       </c>
-      <c r="I41" s="41"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="40"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
       <c r="M41" s="21"/>
       <c r="N41" s="32">
         <f>_input!$H18</f>
@@ -3166,21 +3171,21 @@
         <v>88</v>
       </c>
       <c r="B42" s="22"/>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="40">
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="39">
         <f>_input!$B19</f>
         <v>3344110</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
       <c r="M42" s="21"/>
       <c r="N42" s="32">
         <f>_input!$H19</f>
@@ -3230,21 +3235,21 @@
         <v>88</v>
       </c>
       <c r="B43" s="22"/>
-      <c r="C43" s="42" t="s">
+      <c r="C43" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="40">
+      <c r="D43" s="37"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="39">
         <f>_input!$B20</f>
         <v>3344110</v>
       </c>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
-      <c r="L43" s="41"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
       <c r="M43" s="21"/>
       <c r="N43" s="32">
         <f>_input!$H20</f>
@@ -3294,21 +3299,21 @@
         <v>88</v>
       </c>
       <c r="B44" s="22"/>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="40">
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="39">
         <f>_input!$B21</f>
         <v>3344110</v>
       </c>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
       <c r="M44" s="21"/>
       <c r="N44" s="32">
         <f>_input!$H21</f>
@@ -3358,21 +3363,21 @@
         <v>88</v>
       </c>
       <c r="B45" s="22"/>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="40">
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="39">
         <f>_input!$B22</f>
         <v>3344110</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
       <c r="M45" s="21"/>
       <c r="N45" s="32">
         <f>_input!$H22</f>
@@ -3422,21 +3427,21 @@
         <v>88</v>
       </c>
       <c r="B46" s="22"/>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="40">
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39">
         <f>_input!$B23</f>
         <v>3344110</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
       <c r="M46" s="21"/>
       <c r="N46" s="32">
         <f>_input!$H23</f>
@@ -3486,21 +3491,21 @@
         <v>88</v>
       </c>
       <c r="B47" s="22"/>
-      <c r="C47" s="42" t="s">
+      <c r="C47" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="40">
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="39">
         <f>_input!$B24</f>
         <v>2144110</v>
       </c>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="41"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
       <c r="M47" s="21"/>
       <c r="N47" s="32">
         <f>_input!$H24</f>
@@ -3550,21 +3555,21 @@
         <v>88</v>
       </c>
       <c r="B48" s="22"/>
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="42"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="40">
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="39">
         <f>_input!$B25</f>
         <v>3344110</v>
       </c>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="41"/>
-      <c r="L48" s="41"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
       <c r="M48" s="21"/>
       <c r="N48" s="32">
         <f>_input!$H25</f>
@@ -3609,26 +3614,26 @@
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:29" ht="15" customHeight="1">
+    <row r="49" spans="1:30" ht="15" customHeight="1">
       <c r="A49" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B49" s="22"/>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="42"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="40">
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="39">
         <f>_input!$B26</f>
         <v>3344110</v>
       </c>
-      <c r="I49" s="41"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41"/>
-      <c r="L49" s="41"/>
+      <c r="I49" s="40"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="40"/>
+      <c r="L49" s="40"/>
       <c r="M49" s="21"/>
       <c r="N49" s="32">
         <f>_input!$H26</f>
@@ -3673,26 +3678,26 @@
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:29" ht="15" customHeight="1">
+    <row r="50" spans="1:30" ht="15" customHeight="1">
       <c r="A50" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B50" s="22"/>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="40">
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="39">
         <f>_input!$B27</f>
         <v>3344110</v>
       </c>
-      <c r="I50" s="41"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="41"/>
-      <c r="L50" s="41"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+      <c r="K50" s="40"/>
+      <c r="L50" s="40"/>
       <c r="M50" s="21"/>
       <c r="N50" s="32">
         <f>_input!$H27</f>
@@ -3737,26 +3742,26 @@
         <v>2.9000371876537478E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:29" ht="15" customHeight="1">
+    <row r="51" spans="1:30" ht="15" customHeight="1">
       <c r="A51" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B51" s="22"/>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="42"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="40">
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="39">
         <f>_input!$B28</f>
         <v>3344110</v>
       </c>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
       <c r="M51" s="21"/>
       <c r="N51" s="32">
         <f>_input!$H28</f>
@@ -3801,21 +3806,13 @@
         <v>4.0339841465387494E-2</v>
       </c>
     </row>
+    <row r="52" spans="1:30">
+      <c r="AD52" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="H51:L51"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
     <mergeCell ref="C37:G37"/>
     <mergeCell ref="C38:G38"/>
     <mergeCell ref="C39:G39"/>
@@ -3827,8 +3824,15 @@
     <mergeCell ref="H38:L38"/>
     <mergeCell ref="H39:L39"/>
     <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
     <mergeCell ref="H43:L43"/>
     <mergeCell ref="H44:L44"/>
     <mergeCell ref="H45:L45"/>
@@ -3836,6 +3840,10 @@
     <mergeCell ref="H47:L47"/>
     <mergeCell ref="H48:L48"/>
     <mergeCell ref="H49:L49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="H51:L51"/>
     <mergeCell ref="C44:G44"/>
     <mergeCell ref="C45:G45"/>
     <mergeCell ref="C46:G46"/>
@@ -3847,6 +3855,19 @@
     <mergeCell ref="V32:Y32"/>
     <mergeCell ref="N35:Q35"/>
     <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="V38:Y38"/>
+    <mergeCell ref="V39:Y39"/>
+    <mergeCell ref="V40:Y40"/>
+    <mergeCell ref="V41:Y41"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="V33:Y33"/>
+    <mergeCell ref="V34:Y34"/>
+    <mergeCell ref="V35:Y35"/>
+    <mergeCell ref="V36:Y36"/>
+    <mergeCell ref="V37:Y37"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H42:L42"/>
     <mergeCell ref="V29:Y29"/>
     <mergeCell ref="C48:G48"/>
     <mergeCell ref="N37:Q37"/>
@@ -3871,17 +3892,6 @@
     <mergeCell ref="N32:Q32"/>
     <mergeCell ref="V43:Y43"/>
     <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="V38:Y38"/>
-    <mergeCell ref="V39:Y39"/>
-    <mergeCell ref="V40:Y40"/>
-    <mergeCell ref="V41:Y41"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="V33:Y33"/>
-    <mergeCell ref="V34:Y34"/>
-    <mergeCell ref="V35:Y35"/>
-    <mergeCell ref="V36:Y36"/>
-    <mergeCell ref="V37:Y37"/>
-    <mergeCell ref="N34:Q34"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B24:I24"/>
@@ -4083,7 +4093,9 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>

</xml_diff>

<commit_message>
update chart x-series from 0:00 .... 23:00 to 1:00 ... 24:00
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="trend" sheetId="5" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="93">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -417,6 +417,10 @@
   </si>
   <si>
     <t>downloadFileName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -960,27 +964,66 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -989,45 +1032,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1035,23 +1039,6 @@
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1121,6 +1108,23 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1239,80 +1243,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1415,80 +1419,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1591,80 +1595,80 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>_input!$A$5:$A$28</c:f>
+              <c:f>_input!$E$5:$E$28</c:f>
               <c:strCache>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0:00</c:v>
+                  <c:v>1:00</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1:00</c:v>
+                  <c:v>2:00</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2:00</c:v>
+                  <c:v>3:00</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3:00</c:v>
+                  <c:v>4:00</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4:00</c:v>
+                  <c:v>5:00</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5:00</c:v>
+                  <c:v>6:00</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6:00</c:v>
+                  <c:v>7:00</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7:00</c:v>
+                  <c:v>8:00</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8:00</c:v>
+                  <c:v>9:00</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9:00</c:v>
+                  <c:v>10:00</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10:00</c:v>
+                  <c:v>11:00</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11:00</c:v>
+                  <c:v>12:00</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12:00</c:v>
+                  <c:v>13:00</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13:00</c:v>
+                  <c:v>14:00</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14:00</c:v>
+                  <c:v>15:00</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15:00</c:v>
+                  <c:v>16:00</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16:00</c:v>
+                  <c:v>17:00</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17:00</c:v>
+                  <c:v>18:00</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18:00</c:v>
+                  <c:v>19:00</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19:00</c:v>
+                  <c:v>20:00</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20:00</c:v>
+                  <c:v>21:00</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21:00</c:v>
+                  <c:v>22:00</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22:00</c:v>
+                  <c:v>23:00</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23:00</c:v>
+                  <c:v>24:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1752,11 +1756,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78867456"/>
-        <c:axId val="78889728"/>
+        <c:axId val="80636928"/>
+        <c:axId val="80655104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78867456"/>
+        <c:axId val="80636928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1765,14 +1769,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78889728"/>
+        <c:crossAx val="80655104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78889728"/>
+        <c:axId val="80655104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +1785,7 @@
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78867456"/>
+        <c:crossAx val="80636928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,7 +1803,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000888" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000888" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000899" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000899" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1846,15 +1850,15 @@
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
-    <tableColumn id="3" name="值" dataDxfId="0">
+    <tableColumn id="3" name="值" dataDxfId="4">
       <calculatedColumnFormula>#REF!</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="类型" dataDxfId="4"/>
-    <tableColumn id="5" name="依赖关系" dataDxfId="3">
+    <tableColumn id="4" name="类型" dataDxfId="3"/>
+    <tableColumn id="5" name="依赖关系" dataDxfId="2">
       <calculatedColumnFormula>$B8</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="源" dataDxfId="2"/>
-    <tableColumn id="7" name="格式" dataDxfId="1"/>
+    <tableColumn id="6" name="源" dataDxfId="1"/>
+    <tableColumn id="7" name="格式" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2147,9 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:I24"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
   <cols>
@@ -2173,29 +2175,29 @@
       <c r="R1" s="4"/>
     </row>
     <row r="2" spans="2:18">
-      <c r="B2" s="38" t="str">
+      <c r="B2" s="34" t="str">
         <f>_input!$A2&amp;"+"&amp;_input!$A3&amp;"+趋势图"</f>
         <v>商业产品线+分析指标+趋势图</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
       <c r="R2" s="4"/>
     </row>
     <row r="3" spans="2:18">
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="2:18">
-      <c r="B4" s="37" t="str">
+      <c r="B4" s="33" t="str">
         <f>_input!$B3</f>
         <v>点击消费</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="2:18" ht="3" customHeight="1">
@@ -2256,17 +2258,17 @@
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:29">
-      <c r="B24" s="38" t="str">
+      <c r="B24" s="34" t="str">
         <f>_input!$B3&amp;"分小时数据表"</f>
         <v>点击消费分小时数据表</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
       <c r="R24" s="4"/>
       <c r="X24" t="s">
         <v>30</v>
@@ -2304,71 +2306,71 @@
       <c r="AC26" s="18"/>
     </row>
     <row r="27" spans="1:29" ht="35.25" customHeight="1">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42" t="s">
+      <c r="C27" s="35"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="34" t="s">
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-      <c r="R27" s="35"/>
-      <c r="S27" s="35"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="34" t="s">
+      <c r="O27" s="48"/>
+      <c r="P27" s="48"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="48"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="48"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="W27" s="35"/>
-      <c r="X27" s="35"/>
-      <c r="Y27" s="35"/>
-      <c r="Z27" s="35"/>
-      <c r="AA27" s="35"/>
-      <c r="AB27" s="35"/>
-      <c r="AC27" s="36"/>
+      <c r="W27" s="48"/>
+      <c r="X27" s="48"/>
+      <c r="Y27" s="48"/>
+      <c r="Z27" s="48"/>
+      <c r="AA27" s="48"/>
+      <c r="AB27" s="48"/>
+      <c r="AC27" s="49"/>
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1">
       <c r="A28" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B28" s="22"/>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="27">
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="45">
         <f>_input!$B5</f>
         <v>3344110</v>
       </c>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
       <c r="M28" s="21"/>
-      <c r="N28" s="32">
+      <c r="N28" s="38">
         <f>_input!$H5</f>
         <v>120000</v>
       </c>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
       <c r="R28" s="19" t="s">
         <v>61</v>
       </c>
@@ -2383,13 +2385,13 @@
         <f>_input!$H5</f>
         <v>120000</v>
       </c>
-      <c r="V28" s="31">
+      <c r="V28" s="40">
         <f>_input!$I5</f>
         <v>9670</v>
       </c>
-      <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="31"/>
+      <c r="W28" s="40"/>
+      <c r="X28" s="40"/>
+      <c r="Y28" s="40"/>
       <c r="Z28" s="19" t="s">
         <v>61</v>
       </c>
@@ -2410,29 +2412,29 @@
         <v>88</v>
       </c>
       <c r="B29" s="22"/>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="27">
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45">
         <f>_input!$B6</f>
         <v>3323110</v>
       </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
       <c r="M29" s="21"/>
-      <c r="N29" s="32">
+      <c r="N29" s="38">
         <f>_input!$H6</f>
         <v>-1020000</v>
       </c>
-      <c r="O29" s="33"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="33"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
       <c r="R29" s="19" t="s">
         <v>61</v>
       </c>
@@ -2447,13 +2449,13 @@
         <f>_input!$H6</f>
         <v>-1020000</v>
       </c>
-      <c r="V29" s="31">
+      <c r="V29" s="40">
         <f>_input!$I6</f>
         <v>-330</v>
       </c>
-      <c r="W29" s="31"/>
-      <c r="X29" s="31"/>
-      <c r="Y29" s="31"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
       <c r="Z29" s="19" t="s">
         <v>61</v>
       </c>
@@ -2474,29 +2476,29 @@
         <v>88</v>
       </c>
       <c r="B30" s="22"/>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="27">
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="45">
         <f>_input!$B7</f>
         <v>3344110</v>
       </c>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
       <c r="M30" s="21"/>
-      <c r="N30" s="32">
+      <c r="N30" s="38">
         <f>_input!$H7</f>
         <v>120000</v>
       </c>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
       <c r="R30" s="19" t="s">
         <v>61</v>
       </c>
@@ -2511,13 +2513,13 @@
         <f>_input!$H7</f>
         <v>120000</v>
       </c>
-      <c r="V30" s="31">
+      <c r="V30" s="40">
         <f>_input!$I7</f>
         <v>19670</v>
       </c>
-      <c r="W30" s="31"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
+      <c r="W30" s="40"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="40"/>
       <c r="Z30" s="19" t="s">
         <v>61</v>
       </c>
@@ -2538,29 +2540,29 @@
         <v>88</v>
       </c>
       <c r="B31" s="22"/>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="27">
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="45">
         <f>_input!$B8</f>
         <v>3344110</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
       <c r="M31" s="21"/>
-      <c r="N31" s="32">
+      <c r="N31" s="38">
         <f>_input!$H8</f>
         <v>120000</v>
       </c>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
       <c r="R31" s="19" t="s">
         <v>61</v>
       </c>
@@ -2575,13 +2577,13 @@
         <f>_input!$H8</f>
         <v>120000</v>
       </c>
-      <c r="V31" s="31">
+      <c r="V31" s="40">
         <f>_input!$I8</f>
         <v>9670</v>
       </c>
-      <c r="W31" s="31"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="31"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
       <c r="Z31" s="19" t="s">
         <v>61</v>
       </c>
@@ -2602,29 +2604,29 @@
         <v>88</v>
       </c>
       <c r="B32" s="22"/>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="27">
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="45">
         <f>_input!$B9</f>
         <v>3344110</v>
       </c>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
       <c r="M32" s="21"/>
-      <c r="N32" s="32">
+      <c r="N32" s="38">
         <f>_input!$H9</f>
         <v>-320000</v>
       </c>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="33"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
       <c r="R32" s="19" t="s">
         <v>61</v>
       </c>
@@ -2639,13 +2641,13 @@
         <f>_input!$H9</f>
         <v>-320000</v>
       </c>
-      <c r="V32" s="31">
+      <c r="V32" s="40">
         <f>_input!$I9</f>
         <v>99670</v>
       </c>
-      <c r="W32" s="31"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="31"/>
+      <c r="W32" s="40"/>
+      <c r="X32" s="40"/>
+      <c r="Y32" s="40"/>
       <c r="Z32" s="19" t="s">
         <v>61</v>
       </c>
@@ -2666,29 +2668,29 @@
         <v>88</v>
       </c>
       <c r="B33" s="22"/>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="27">
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="45">
         <f>_input!$B10</f>
         <v>3344110</v>
       </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
       <c r="M33" s="21"/>
-      <c r="N33" s="32">
+      <c r="N33" s="38">
         <f>_input!$H10</f>
         <v>120000</v>
       </c>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
       <c r="R33" s="19" t="s">
         <v>61</v>
       </c>
@@ -2703,13 +2705,13 @@
         <f>_input!$H10</f>
         <v>120000</v>
       </c>
-      <c r="V33" s="31">
+      <c r="V33" s="40">
         <f>_input!$I10</f>
         <v>9670</v>
       </c>
-      <c r="W33" s="31"/>
-      <c r="X33" s="31"/>
-      <c r="Y33" s="31"/>
+      <c r="W33" s="40"/>
+      <c r="X33" s="40"/>
+      <c r="Y33" s="40"/>
       <c r="Z33" s="19" t="s">
         <v>61</v>
       </c>
@@ -2730,29 +2732,29 @@
         <v>88</v>
       </c>
       <c r="B34" s="22"/>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="27">
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="45">
         <f>_input!$B11</f>
         <v>4344110</v>
       </c>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
       <c r="M34" s="21"/>
-      <c r="N34" s="32">
+      <c r="N34" s="38">
         <f>_input!$H11</f>
         <v>20000</v>
       </c>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
       <c r="R34" s="19" t="s">
         <v>61</v>
       </c>
@@ -2767,13 +2769,13 @@
         <f>_input!$H11</f>
         <v>20000</v>
       </c>
-      <c r="V34" s="31">
+      <c r="V34" s="40">
         <f>_input!$I11</f>
         <v>1009670</v>
       </c>
-      <c r="W34" s="31"/>
-      <c r="X34" s="31"/>
-      <c r="Y34" s="31"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
       <c r="Z34" s="19" t="s">
         <v>61</v>
       </c>
@@ -2794,29 +2796,29 @@
         <v>88</v>
       </c>
       <c r="B35" s="22"/>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="27">
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="45">
         <f>_input!$B12</f>
         <v>3344110</v>
       </c>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="28"/>
+      <c r="I35" s="46"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
       <c r="M35" s="21"/>
-      <c r="N35" s="32">
+      <c r="N35" s="38">
         <f>_input!$H12</f>
         <v>120000</v>
       </c>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
       <c r="R35" s="19" t="s">
         <v>61</v>
       </c>
@@ -2831,13 +2833,13 @@
         <f>_input!$H12</f>
         <v>120000</v>
       </c>
-      <c r="V35" s="31">
+      <c r="V35" s="40">
         <f>_input!$I12</f>
         <v>-210330</v>
       </c>
-      <c r="W35" s="31"/>
-      <c r="X35" s="31"/>
-      <c r="Y35" s="31"/>
+      <c r="W35" s="40"/>
+      <c r="X35" s="40"/>
+      <c r="Y35" s="40"/>
       <c r="Z35" s="19" t="s">
         <v>61</v>
       </c>
@@ -2858,29 +2860,29 @@
         <v>88</v>
       </c>
       <c r="B36" s="22"/>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="27">
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="45">
         <f>_input!$B13</f>
         <v>3344110</v>
       </c>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="28"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
       <c r="M36" s="21"/>
-      <c r="N36" s="32">
+      <c r="N36" s="38">
         <f>_input!$H13</f>
         <v>120000</v>
       </c>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
       <c r="R36" s="19" t="s">
         <v>61</v>
       </c>
@@ -2895,13 +2897,13 @@
         <f>_input!$H13</f>
         <v>120000</v>
       </c>
-      <c r="V36" s="31">
+      <c r="V36" s="40">
         <f>_input!$I13</f>
         <v>-330330</v>
       </c>
-      <c r="W36" s="31"/>
-      <c r="X36" s="31"/>
-      <c r="Y36" s="31"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
       <c r="Z36" s="19" t="s">
         <v>61</v>
       </c>
@@ -2922,29 +2924,29 @@
         <v>88</v>
       </c>
       <c r="B37" s="22"/>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="27">
+      <c r="D37" s="43"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="45">
         <f>_input!$B14</f>
         <v>3344110</v>
       </c>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
       <c r="M37" s="21"/>
-      <c r="N37" s="32">
+      <c r="N37" s="38">
         <f>_input!$H14</f>
         <v>120000</v>
       </c>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
+      <c r="O37" s="39"/>
+      <c r="P37" s="39"/>
+      <c r="Q37" s="39"/>
       <c r="R37" s="19" t="s">
         <v>61</v>
       </c>
@@ -2959,13 +2961,13 @@
         <f>_input!$H14</f>
         <v>120000</v>
       </c>
-      <c r="V37" s="31">
+      <c r="V37" s="40">
         <f>_input!$I14</f>
         <v>9670</v>
       </c>
-      <c r="W37" s="31"/>
-      <c r="X37" s="31"/>
-      <c r="Y37" s="31"/>
+      <c r="W37" s="40"/>
+      <c r="X37" s="40"/>
+      <c r="Y37" s="40"/>
       <c r="Z37" s="19" t="s">
         <v>61</v>
       </c>
@@ -2986,29 +2988,29 @@
         <v>88</v>
       </c>
       <c r="B38" s="22"/>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="27">
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45">
         <f>_input!$B15</f>
         <v>3344110</v>
       </c>
-      <c r="I38" s="28"/>
-      <c r="J38" s="28"/>
-      <c r="K38" s="28"/>
-      <c r="L38" s="28"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
       <c r="M38" s="21"/>
-      <c r="N38" s="32">
+      <c r="N38" s="38">
         <f>_input!$H15</f>
         <v>-180000</v>
       </c>
-      <c r="O38" s="33"/>
-      <c r="P38" s="33"/>
-      <c r="Q38" s="33"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
       <c r="R38" s="19" t="s">
         <v>61</v>
       </c>
@@ -3023,13 +3025,13 @@
         <f>_input!$H15</f>
         <v>-180000</v>
       </c>
-      <c r="V38" s="31">
+      <c r="V38" s="40">
         <f>_input!$I15</f>
         <v>-200330</v>
       </c>
-      <c r="W38" s="31"/>
-      <c r="X38" s="31"/>
-      <c r="Y38" s="31"/>
+      <c r="W38" s="40"/>
+      <c r="X38" s="40"/>
+      <c r="Y38" s="40"/>
       <c r="Z38" s="19" t="s">
         <v>61</v>
       </c>
@@ -3050,29 +3052,29 @@
         <v>88</v>
       </c>
       <c r="B39" s="22"/>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="27">
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="45">
         <f>_input!$B16</f>
         <v>3344110</v>
       </c>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
       <c r="M39" s="21"/>
-      <c r="N39" s="32">
+      <c r="N39" s="38">
         <f>_input!$H16</f>
         <v>120000</v>
       </c>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="39"/>
+      <c r="Q39" s="39"/>
       <c r="R39" s="19" t="s">
         <v>61</v>
       </c>
@@ -3087,13 +3089,13 @@
         <f>_input!$H16</f>
         <v>120000</v>
       </c>
-      <c r="V39" s="31">
+      <c r="V39" s="40">
         <f>_input!$I16</f>
         <v>9670</v>
       </c>
-      <c r="W39" s="31"/>
-      <c r="X39" s="31"/>
-      <c r="Y39" s="31"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
       <c r="Z39" s="19" t="s">
         <v>61</v>
       </c>
@@ -3114,29 +3116,29 @@
         <v>88</v>
       </c>
       <c r="B40" s="22"/>
-      <c r="C40" s="29" t="s">
+      <c r="C40" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="27">
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="45">
         <f>_input!$B17</f>
         <v>3344110</v>
       </c>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
       <c r="M40" s="21"/>
-      <c r="N40" s="32">
+      <c r="N40" s="38">
         <f>_input!$H17</f>
         <v>120000</v>
       </c>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
+      <c r="O40" s="39"/>
+      <c r="P40" s="39"/>
+      <c r="Q40" s="39"/>
       <c r="R40" s="19" t="s">
         <v>61</v>
       </c>
@@ -3151,13 +3153,13 @@
         <f>_input!$H17</f>
         <v>120000</v>
       </c>
-      <c r="V40" s="31">
+      <c r="V40" s="40">
         <f>_input!$I17</f>
         <v>9670</v>
       </c>
-      <c r="W40" s="31"/>
-      <c r="X40" s="31"/>
-      <c r="Y40" s="31"/>
+      <c r="W40" s="40"/>
+      <c r="X40" s="40"/>
+      <c r="Y40" s="40"/>
       <c r="Z40" s="19" t="s">
         <v>61</v>
       </c>
@@ -3178,29 +3180,29 @@
         <v>88</v>
       </c>
       <c r="B41" s="22"/>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="27">
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="45">
         <f>_input!$B18</f>
         <v>3484110</v>
       </c>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
       <c r="M41" s="21"/>
-      <c r="N41" s="32">
+      <c r="N41" s="38">
         <f>_input!$H18</f>
         <v>260000</v>
       </c>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="39"/>
       <c r="R41" s="19" t="s">
         <v>61</v>
       </c>
@@ -3215,13 +3217,13 @@
         <f>_input!$H18</f>
         <v>260000</v>
       </c>
-      <c r="V41" s="31">
+      <c r="V41" s="40">
         <f>_input!$I18</f>
         <v>139670</v>
       </c>
-      <c r="W41" s="31"/>
-      <c r="X41" s="31"/>
-      <c r="Y41" s="31"/>
+      <c r="W41" s="40"/>
+      <c r="X41" s="40"/>
+      <c r="Y41" s="40"/>
       <c r="Z41" s="19" t="s">
         <v>61</v>
       </c>
@@ -3242,29 +3244,29 @@
         <v>88</v>
       </c>
       <c r="B42" s="22"/>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="27">
+      <c r="D42" s="43"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="45">
         <f>_input!$B19</f>
         <v>3344110</v>
       </c>
-      <c r="I42" s="28"/>
-      <c r="J42" s="28"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="28"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
       <c r="M42" s="21"/>
-      <c r="N42" s="32">
+      <c r="N42" s="38">
         <f>_input!$H19</f>
         <v>120000</v>
       </c>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
-      <c r="Q42" s="33"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
       <c r="R42" s="19" t="s">
         <v>61</v>
       </c>
@@ -3279,13 +3281,13 @@
         <f>_input!$H19</f>
         <v>120000</v>
       </c>
-      <c r="V42" s="31">
+      <c r="V42" s="40">
         <f>_input!$I19</f>
         <v>9670</v>
       </c>
-      <c r="W42" s="31"/>
-      <c r="X42" s="31"/>
-      <c r="Y42" s="31"/>
+      <c r="W42" s="40"/>
+      <c r="X42" s="40"/>
+      <c r="Y42" s="40"/>
       <c r="Z42" s="19" t="s">
         <v>61</v>
       </c>
@@ -3306,29 +3308,29 @@
         <v>88</v>
       </c>
       <c r="B43" s="22"/>
-      <c r="C43" s="29" t="s">
+      <c r="C43" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="27">
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="45">
         <f>_input!$B20</f>
         <v>3344110</v>
       </c>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="28"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
       <c r="M43" s="21"/>
-      <c r="N43" s="32">
+      <c r="N43" s="38">
         <f>_input!$H20</f>
         <v>120000</v>
       </c>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
+      <c r="O43" s="39"/>
+      <c r="P43" s="39"/>
+      <c r="Q43" s="39"/>
       <c r="R43" s="19" t="s">
         <v>61</v>
       </c>
@@ -3343,13 +3345,13 @@
         <f>_input!$H20</f>
         <v>120000</v>
       </c>
-      <c r="V43" s="31">
+      <c r="V43" s="40">
         <f>_input!$I20</f>
         <v>-200330</v>
       </c>
-      <c r="W43" s="31"/>
-      <c r="X43" s="31"/>
-      <c r="Y43" s="31"/>
+      <c r="W43" s="40"/>
+      <c r="X43" s="40"/>
+      <c r="Y43" s="40"/>
       <c r="Z43" s="19" t="s">
         <v>61</v>
       </c>
@@ -3370,29 +3372,29 @@
         <v>88</v>
       </c>
       <c r="B44" s="22"/>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="27">
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="45">
         <f>_input!$B21</f>
         <v>3344110</v>
       </c>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
       <c r="M44" s="21"/>
-      <c r="N44" s="32">
+      <c r="N44" s="38">
         <f>_input!$H21</f>
         <v>-90000</v>
       </c>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
+      <c r="O44" s="39"/>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
       <c r="R44" s="19" t="s">
         <v>61</v>
       </c>
@@ -3407,13 +3409,13 @@
         <f>_input!$H21</f>
         <v>-90000</v>
       </c>
-      <c r="V44" s="31">
+      <c r="V44" s="40">
         <f>_input!$I21</f>
         <v>9670</v>
       </c>
-      <c r="W44" s="31"/>
-      <c r="X44" s="31"/>
-      <c r="Y44" s="31"/>
+      <c r="W44" s="40"/>
+      <c r="X44" s="40"/>
+      <c r="Y44" s="40"/>
       <c r="Z44" s="19" t="s">
         <v>61</v>
       </c>
@@ -3434,29 +3436,29 @@
         <v>88</v>
       </c>
       <c r="B45" s="22"/>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="27">
+      <c r="D45" s="43"/>
+      <c r="E45" s="43"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="45">
         <f>_input!$B22</f>
         <v>3344110</v>
       </c>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="28"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
       <c r="M45" s="21"/>
-      <c r="N45" s="32">
+      <c r="N45" s="38">
         <f>_input!$H22</f>
         <v>120000</v>
       </c>
-      <c r="O45" s="33"/>
-      <c r="P45" s="33"/>
-      <c r="Q45" s="33"/>
+      <c r="O45" s="39"/>
+      <c r="P45" s="39"/>
+      <c r="Q45" s="39"/>
       <c r="R45" s="19" t="s">
         <v>61</v>
       </c>
@@ -3471,13 +3473,13 @@
         <f>_input!$H22</f>
         <v>120000</v>
       </c>
-      <c r="V45" s="31">
+      <c r="V45" s="40">
         <f>_input!$I22</f>
         <v>9670</v>
       </c>
-      <c r="W45" s="31"/>
-      <c r="X45" s="31"/>
-      <c r="Y45" s="31"/>
+      <c r="W45" s="40"/>
+      <c r="X45" s="40"/>
+      <c r="Y45" s="40"/>
       <c r="Z45" s="19" t="s">
         <v>61</v>
       </c>
@@ -3498,29 +3500,29 @@
         <v>88</v>
       </c>
       <c r="B46" s="22"/>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="27">
+      <c r="D46" s="43"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="45">
         <f>_input!$B23</f>
         <v>3344110</v>
       </c>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
       <c r="M46" s="21"/>
-      <c r="N46" s="32">
+      <c r="N46" s="38">
         <f>_input!$H23</f>
         <v>120000</v>
       </c>
-      <c r="O46" s="33"/>
-      <c r="P46" s="33"/>
-      <c r="Q46" s="33"/>
+      <c r="O46" s="39"/>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
       <c r="R46" s="19" t="s">
         <v>61</v>
       </c>
@@ -3535,13 +3537,13 @@
         <f>_input!$H23</f>
         <v>120000</v>
       </c>
-      <c r="V46" s="31">
+      <c r="V46" s="40">
         <f>_input!$I23</f>
         <v>9670</v>
       </c>
-      <c r="W46" s="31"/>
-      <c r="X46" s="31"/>
-      <c r="Y46" s="31"/>
+      <c r="W46" s="40"/>
+      <c r="X46" s="40"/>
+      <c r="Y46" s="40"/>
       <c r="Z46" s="19" t="s">
         <v>61</v>
       </c>
@@ -3562,29 +3564,29 @@
         <v>88</v>
       </c>
       <c r="B47" s="22"/>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="27">
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="45">
         <f>_input!$B24</f>
         <v>2144110</v>
       </c>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
       <c r="M47" s="21"/>
-      <c r="N47" s="32">
+      <c r="N47" s="38">
         <f>_input!$H24</f>
         <v>-1080000</v>
       </c>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="33"/>
+      <c r="O47" s="39"/>
+      <c r="P47" s="39"/>
+      <c r="Q47" s="39"/>
       <c r="R47" s="19" t="s">
         <v>61</v>
       </c>
@@ -3599,13 +3601,13 @@
         <f>_input!$H24</f>
         <v>-1080000</v>
       </c>
-      <c r="V47" s="31">
+      <c r="V47" s="40">
         <f>_input!$I24</f>
         <v>-1190330</v>
       </c>
-      <c r="W47" s="31"/>
-      <c r="X47" s="31"/>
-      <c r="Y47" s="31"/>
+      <c r="W47" s="40"/>
+      <c r="X47" s="40"/>
+      <c r="Y47" s="40"/>
       <c r="Z47" s="19" t="s">
         <v>61</v>
       </c>
@@ -3626,29 +3628,29 @@
         <v>88</v>
       </c>
       <c r="B48" s="22"/>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="27">
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="45">
         <f>_input!$B25</f>
         <v>3344110</v>
       </c>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
       <c r="M48" s="21"/>
-      <c r="N48" s="32">
+      <c r="N48" s="38">
         <f>_input!$H25</f>
         <v>120000</v>
       </c>
-      <c r="O48" s="33"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
+      <c r="O48" s="39"/>
+      <c r="P48" s="39"/>
+      <c r="Q48" s="39"/>
       <c r="R48" s="19" t="s">
         <v>61</v>
       </c>
@@ -3663,13 +3665,13 @@
         <f>_input!$H25</f>
         <v>120000</v>
       </c>
-      <c r="V48" s="31">
+      <c r="V48" s="40">
         <f>_input!$I25</f>
         <v>9670</v>
       </c>
-      <c r="W48" s="31"/>
-      <c r="X48" s="31"/>
-      <c r="Y48" s="31"/>
+      <c r="W48" s="40"/>
+      <c r="X48" s="40"/>
+      <c r="Y48" s="40"/>
       <c r="Z48" s="19" t="s">
         <v>61</v>
       </c>
@@ -3690,29 +3692,29 @@
         <v>88</v>
       </c>
       <c r="B49" s="22"/>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="27">
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="45">
         <f>_input!$B26</f>
         <v>3344110</v>
       </c>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
       <c r="M49" s="21"/>
-      <c r="N49" s="32">
+      <c r="N49" s="38">
         <f>_input!$H26</f>
         <v>120000</v>
       </c>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
+      <c r="O49" s="39"/>
+      <c r="P49" s="39"/>
+      <c r="Q49" s="39"/>
       <c r="R49" s="19" t="s">
         <v>61</v>
       </c>
@@ -3727,13 +3729,13 @@
         <f>_input!$H26</f>
         <v>120000</v>
       </c>
-      <c r="V49" s="31">
+      <c r="V49" s="40">
         <f>_input!$I26</f>
         <v>9670</v>
       </c>
-      <c r="W49" s="31"/>
-      <c r="X49" s="31"/>
-      <c r="Y49" s="31"/>
+      <c r="W49" s="40"/>
+      <c r="X49" s="40"/>
+      <c r="Y49" s="40"/>
       <c r="Z49" s="19" t="s">
         <v>61</v>
       </c>
@@ -3754,29 +3756,29 @@
         <v>88</v>
       </c>
       <c r="B50" s="22"/>
-      <c r="C50" s="29" t="s">
+      <c r="C50" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="27">
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="45">
         <f>_input!$B27</f>
         <v>3344110</v>
       </c>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="28"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
       <c r="M50" s="21"/>
-      <c r="N50" s="32">
+      <c r="N50" s="38">
         <f>_input!$H27</f>
         <v>-650000</v>
       </c>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39"/>
+      <c r="Q50" s="39"/>
       <c r="R50" s="19" t="s">
         <v>61</v>
       </c>
@@ -3791,13 +3793,13 @@
         <f>_input!$H27</f>
         <v>-650000</v>
       </c>
-      <c r="V50" s="31">
+      <c r="V50" s="40">
         <f>_input!$I27</f>
         <v>9670</v>
       </c>
-      <c r="W50" s="31"/>
-      <c r="X50" s="31"/>
-      <c r="Y50" s="31"/>
+      <c r="W50" s="40"/>
+      <c r="X50" s="40"/>
+      <c r="Y50" s="40"/>
       <c r="Z50" s="19" t="s">
         <v>61</v>
       </c>
@@ -3818,29 +3820,29 @@
         <v>88</v>
       </c>
       <c r="B51" s="22"/>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="27">
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="45">
         <f>_input!$B28</f>
         <v>3344110</v>
       </c>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
       <c r="M51" s="21"/>
-      <c r="N51" s="32">
+      <c r="N51" s="38">
         <f>_input!$H28</f>
         <v>120000</v>
       </c>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="33"/>
+      <c r="O51" s="39"/>
+      <c r="P51" s="39"/>
+      <c r="Q51" s="39"/>
       <c r="R51" s="19" t="s">
         <v>61</v>
       </c>
@@ -3855,13 +3857,13 @@
         <f>_input!$H28</f>
         <v>120000</v>
       </c>
-      <c r="V51" s="31">
+      <c r="V51" s="40">
         <f>_input!$I28</f>
         <v>129670</v>
       </c>
-      <c r="W51" s="31"/>
-      <c r="X51" s="31"/>
-      <c r="Y51" s="31"/>
+      <c r="W51" s="40"/>
+      <c r="X51" s="40"/>
+      <c r="Y51" s="40"/>
       <c r="Z51" s="19" t="s">
         <v>61</v>
       </c>
@@ -3884,6 +3886,85 @@
     </row>
   </sheetData>
   <mergeCells count="103">
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="H49:L49"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="H51:L51"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C45:G45"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="H35:L35"/>
+    <mergeCell ref="H36:L36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="H39:L39"/>
+    <mergeCell ref="H40:L40"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="V30:Y30"/>
+    <mergeCell ref="V31:Y31"/>
+    <mergeCell ref="V32:Y32"/>
+    <mergeCell ref="N35:Q35"/>
+    <mergeCell ref="N36:Q36"/>
+    <mergeCell ref="V38:Y38"/>
+    <mergeCell ref="V39:Y39"/>
+    <mergeCell ref="V40:Y40"/>
+    <mergeCell ref="V41:Y41"/>
+    <mergeCell ref="V42:Y42"/>
+    <mergeCell ref="V33:Y33"/>
+    <mergeCell ref="V34:Y34"/>
+    <mergeCell ref="V35:Y35"/>
+    <mergeCell ref="V36:Y36"/>
+    <mergeCell ref="V37:Y37"/>
+    <mergeCell ref="N34:Q34"/>
+    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="V29:Y29"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="N37:Q37"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="H37:L37"/>
+    <mergeCell ref="N44:Q44"/>
+    <mergeCell ref="N27:U27"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="V27:AC27"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="H30:L30"/>
+    <mergeCell ref="H31:L31"/>
+    <mergeCell ref="H32:L32"/>
+    <mergeCell ref="H33:L33"/>
+    <mergeCell ref="H34:L34"/>
+    <mergeCell ref="N46:Q46"/>
+    <mergeCell ref="N47:Q47"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="N31:Q31"/>
+    <mergeCell ref="N32:Q32"/>
+    <mergeCell ref="V43:Y43"/>
+    <mergeCell ref="V44:Y44"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B24:I24"/>
@@ -3908,85 +3989,6 @@
     <mergeCell ref="N33:Q33"/>
     <mergeCell ref="V28:Y28"/>
     <mergeCell ref="H27:M27"/>
-    <mergeCell ref="V29:Y29"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="H37:L37"/>
-    <mergeCell ref="N44:Q44"/>
-    <mergeCell ref="N27:U27"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="V27:AC27"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="H30:L30"/>
-    <mergeCell ref="H31:L31"/>
-    <mergeCell ref="H32:L32"/>
-    <mergeCell ref="H33:L33"/>
-    <mergeCell ref="H34:L34"/>
-    <mergeCell ref="N46:Q46"/>
-    <mergeCell ref="N47:Q47"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="N29:Q29"/>
-    <mergeCell ref="N30:Q30"/>
-    <mergeCell ref="N31:Q31"/>
-    <mergeCell ref="N32:Q32"/>
-    <mergeCell ref="V43:Y43"/>
-    <mergeCell ref="V44:Y44"/>
-    <mergeCell ref="V42:Y42"/>
-    <mergeCell ref="V33:Y33"/>
-    <mergeCell ref="V34:Y34"/>
-    <mergeCell ref="V35:Y35"/>
-    <mergeCell ref="V36:Y36"/>
-    <mergeCell ref="V37:Y37"/>
-    <mergeCell ref="N34:Q34"/>
-    <mergeCell ref="H41:L41"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="V30:Y30"/>
-    <mergeCell ref="V31:Y31"/>
-    <mergeCell ref="V32:Y32"/>
-    <mergeCell ref="N35:Q35"/>
-    <mergeCell ref="N36:Q36"/>
-    <mergeCell ref="V38:Y38"/>
-    <mergeCell ref="V39:Y39"/>
-    <mergeCell ref="V40:Y40"/>
-    <mergeCell ref="V41:Y41"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
-    <mergeCell ref="H50:L50"/>
-    <mergeCell ref="H51:L51"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C45:G45"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="H35:L35"/>
-    <mergeCell ref="H36:L36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="H39:L39"/>
-    <mergeCell ref="H40:L40"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="H49:L49"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C34:G34"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="C36:G36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="U28:U51">
@@ -4019,7 +4021,7 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -4102,7 +4104,7 @@
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4147,18 +4149,18 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="46" t="str">
+      <c r="C12" s="29" t="str">
         <f>_input!$B2 &amp; "" &amp;_input!$B3&amp; "分小时数据表"</f>
         <v>搜索+推广点击消费分小时数据表</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="48"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4178,9 +4180,7 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -4243,6 +4243,9 @@
       <c r="D5" s="25">
         <v>3334440</v>
       </c>
+      <c r="E5" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" s="17">
         <f>IF($C5=0,0,$B5/$C5-1)</f>
         <v>3.7219573773847658E-2</v>
@@ -4273,6 +4276,9 @@
       <c r="D6" s="25">
         <v>3323440</v>
       </c>
+      <c r="E6" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="F6" s="17">
         <f t="shared" ref="F6:F28" si="0">IF($C6=0,0,$B6/$C6-1)</f>
         <v>-0.23485474694401021</v>
@@ -4303,6 +4309,9 @@
       <c r="D7" s="25">
         <v>3324440</v>
       </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="F7" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4333,6 +4342,9 @@
       <c r="D8" s="25">
         <v>3334440</v>
       </c>
+      <c r="E8" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4363,6 +4375,9 @@
       <c r="D9" s="25">
         <v>3244440</v>
       </c>
+      <c r="E9" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="F9" s="17">
         <f t="shared" si="0"/>
         <v>-8.7333622625958229E-2</v>
@@ -4393,6 +4408,9 @@
       <c r="D10" s="25">
         <v>3334440</v>
       </c>
+      <c r="E10" s="16" t="s">
+        <v>40</v>
+      </c>
       <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4423,6 +4441,9 @@
       <c r="D11" s="25">
         <v>3334440</v>
       </c>
+      <c r="E11" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="F11" s="17">
         <f t="shared" si="0"/>
         <v>4.6252292379240778E-3</v>
@@ -4453,6 +4474,9 @@
       <c r="D12" s="25">
         <v>3554440</v>
       </c>
+      <c r="E12" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4483,6 +4507,9 @@
       <c r="D13" s="25">
         <v>3674440</v>
       </c>
+      <c r="E13" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4513,6 +4540,9 @@
       <c r="D14" s="25">
         <v>3334440</v>
       </c>
+      <c r="E14" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="F14" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4543,6 +4573,9 @@
       <c r="D15" s="25">
         <v>3544440</v>
       </c>
+      <c r="E15" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="F15" s="17">
         <f t="shared" si="0"/>
         <v>-5.1076725754871433E-2</v>
@@ -4573,6 +4606,9 @@
       <c r="D16" s="25">
         <v>3334440</v>
       </c>
+      <c r="E16" s="16" t="s">
+        <v>46</v>
+      </c>
       <c r="F16" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4603,6 +4639,9 @@
       <c r="D17" s="25">
         <v>3334440</v>
       </c>
+      <c r="E17" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="F17" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4633,6 +4672,9 @@
       <c r="D18" s="25">
         <v>3344440</v>
       </c>
+      <c r="E18" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="F18" s="17">
         <f t="shared" si="0"/>
         <v>8.0642409843336704E-2</v>
@@ -4663,6 +4705,9 @@
       <c r="D19" s="25">
         <v>3334440</v>
       </c>
+      <c r="E19" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="F19" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4693,6 +4738,9 @@
       <c r="D20" s="25">
         <v>3544440</v>
       </c>
+      <c r="E20" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="F20" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4723,6 +4771,9 @@
       <c r="D21" s="25">
         <v>3334440</v>
       </c>
+      <c r="E21" s="16" t="s">
+        <v>51</v>
+      </c>
       <c r="F21" s="17">
         <f t="shared" si="0"/>
         <v>-2.6207663703259332E-2</v>
@@ -4753,6 +4804,9 @@
       <c r="D22" s="25">
         <v>3334440</v>
       </c>
+      <c r="E22" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="F22" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4783,6 +4837,9 @@
       <c r="D23" s="25">
         <v>3334440</v>
       </c>
+      <c r="E23" s="16" t="s">
+        <v>53</v>
+      </c>
       <c r="F23" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4813,6 +4870,9 @@
       <c r="D24" s="25">
         <v>3334440</v>
       </c>
+      <c r="E24" s="16" t="s">
+        <v>54</v>
+      </c>
       <c r="F24" s="17">
         <f t="shared" si="0"/>
         <v>-0.33497616396462904</v>
@@ -4843,6 +4903,9 @@
       <c r="D25" s="25">
         <v>3334440</v>
       </c>
+      <c r="E25" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="F25" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4873,6 +4936,9 @@
       <c r="D26" s="25">
         <v>3334440</v>
       </c>
+      <c r="E26" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="F26" s="17">
         <f t="shared" si="0"/>
         <v>3.7219573773847658E-2</v>
@@ -4903,6 +4969,9 @@
       <c r="D27" s="25">
         <v>3334440</v>
       </c>
+      <c r="E27" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="F27" s="17">
         <f t="shared" si="0"/>
         <v>-0.16273963411122883</v>
@@ -4932,6 +5001,9 @@
       </c>
       <c r="D28" s="25">
         <v>3214440</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="F28" s="17">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
update for new compass
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/luopan-trend-rt.xlsx
@@ -1756,11 +1756,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="80636928"/>
-        <c:axId val="80655104"/>
+        <c:axId val="81161600"/>
+        <c:axId val="81179776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80636928"/>
+        <c:axId val="81161600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1769,14 +1769,14 @@
         <c:numFmt formatCode="yyyy/m/d" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80655104"/>
+        <c:crossAx val="81179776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80655104"/>
+        <c:axId val="81179776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,7 +1785,7 @@
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80636928"/>
+        <c:crossAx val="81161600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1803,7 +1803,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000899" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000899" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000921" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000921" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2159,16 +2159,18 @@
     <col min="2" max="2" width="0.75" customWidth="1"/>
     <col min="3" max="12" width="6.125" customWidth="1"/>
     <col min="13" max="13" width="1.125" customWidth="1"/>
-    <col min="14" max="17" width="6.125" customWidth="1"/>
+    <col min="14" max="15" width="5" customWidth="1"/>
+    <col min="16" max="17" width="6.125" customWidth="1"/>
     <col min="18" max="18" width="1.5" customWidth="1"/>
     <col min="19" max="19" width="10.125" customWidth="1"/>
     <col min="20" max="20" width="1.5" customWidth="1"/>
-    <col min="21" max="21" width="2.375" customWidth="1"/>
-    <col min="22" max="25" width="6.125" customWidth="1"/>
+    <col min="21" max="21" width="3.625" customWidth="1"/>
+    <col min="22" max="23" width="5.25" customWidth="1"/>
+    <col min="24" max="25" width="6.125" customWidth="1"/>
     <col min="26" max="26" width="1.5" customWidth="1"/>
     <col min="27" max="27" width="10.125" customWidth="1"/>
     <col min="28" max="28" width="1.5" customWidth="1"/>
-    <col min="29" max="29" width="2.25" customWidth="1"/>
+    <col min="29" max="29" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="3.75" customHeight="1">

</xml_diff>